<commit_message>
Included information on Financial Metrics + Changes to Code
</commit_message>
<xml_diff>
--- a/List of Companies and Sustainability Reports.xlsx
+++ b/List of Companies and Sustainability Reports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy Chia\Documents\GitHub\NLP-SustainabilityReports-FinancialPerformance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA099A28-AFE9-4E07-A794-90118C9FBDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910E520A-C5A9-41C5-A04F-F817005D6278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Companies" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="Files (Original)" sheetId="1" r:id="rId3"/>
     <sheet name="Files (New)" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Files (New)'!$A$1:$E$206</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -57,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1551" uniqueCount="566">
   <si>
     <t>ASCENDAS REAL ESTATE INV TRUST_2015_SUS.pdf</t>
   </si>
@@ -1289,9 +1292,6 @@
     <t>C:\Users\Jeremy Chia\Documents\GitHub\NLP-SustainabilityReports-FinancialPerformance\Sustainability Reports or Annual Reports\KEPPEL DC REIT_2021_SUS.pdf</t>
   </si>
   <si>
-    <t>C:\Users\Jeremy Chia\Documents\GitHub\NLP-SustainabilityReports-FinancialPerformance\Sustainability Reports or Annual Reports\list.csv</t>
-  </si>
-  <si>
     <t>C:\Users\Jeremy Chia\Documents\GitHub\NLP-SustainabilityReports-FinancialPerformance\Sustainability Reports or Annual Reports\MAPLETREE COMMERCIAL TRUST_2015_SUS.pdf</t>
   </si>
   <si>
@@ -1755,6 +1755,9 @@
   </si>
   <si>
     <t>DocumentName</t>
+  </si>
+  <si>
+    <t>Report</t>
   </si>
 </sst>
 </file>
@@ -2322,18 +2325,7 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2357,7 +2349,18 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2381,28 +2384,28 @@
     <tableColumn id="3" xr3:uid="{D0D3DE39-8C3D-484F-B63C-09BB29A1D3A4}" name="Ticker SGX" totalsRowFunction="count">
       <calculatedColumnFormula>TRIM(MID(B2,FIND(":",B2)+1,FIND(")",B2)-FIND(":",B2)-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{614E20B8-97EA-4750-A17D-869D637325FA}" name="2015" dataDxfId="9">
+    <tableColumn id="4" xr3:uid="{614E20B8-97EA-4750-A17D-869D637325FA}" name="2015" dataDxfId="7">
       <calculatedColumnFormula array="1">IFERROR(INDEX('Files (Original)'!$D:$D,MATCH(1,($A2='Files (Original)'!$B:$B)*(_xlfn.NUMBERVALUE(D$1)='Files (Original)'!$C:$C),0)),"Missing")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{0A287D94-DAE8-4091-A28A-33373CC91786}" name="2016" dataDxfId="8">
+    <tableColumn id="5" xr3:uid="{0A287D94-DAE8-4091-A28A-33373CC91786}" name="2016" dataDxfId="6">
       <calculatedColumnFormula array="1">IFERROR(INDEX('Files (Original)'!$D:$D,MATCH(1,($A2='Files (Original)'!$B:$B)*(_xlfn.NUMBERVALUE(E$1)='Files (Original)'!$C:$C),0)),"Missing")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{157DD905-4513-45E9-BC0F-44DBDDB0E97F}" name="2017" dataDxfId="7">
+    <tableColumn id="6" xr3:uid="{157DD905-4513-45E9-BC0F-44DBDDB0E97F}" name="2017" dataDxfId="5">
       <calculatedColumnFormula array="1">IFERROR(INDEX('Files (Original)'!$D:$D,MATCH(1,($A2='Files (Original)'!$B:$B)*(_xlfn.NUMBERVALUE(F$1)='Files (Original)'!$C:$C),0)),"Missing")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5A03B6FD-EBEB-40E7-8A7C-F20E290423E1}" name="2018" dataDxfId="6">
+    <tableColumn id="7" xr3:uid="{5A03B6FD-EBEB-40E7-8A7C-F20E290423E1}" name="2018" dataDxfId="4">
       <calculatedColumnFormula array="1">IFERROR(INDEX('Files (Original)'!$D:$D,MATCH(1,($A2='Files (Original)'!$B:$B)*(_xlfn.NUMBERVALUE(G$1)='Files (Original)'!$C:$C),0)),"Missing")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4A2EB404-117C-4AED-ABED-FC2DC3BD162B}" name="2019" dataDxfId="5">
+    <tableColumn id="8" xr3:uid="{4A2EB404-117C-4AED-ABED-FC2DC3BD162B}" name="2019" dataDxfId="3">
       <calculatedColumnFormula array="1">IFERROR(INDEX('Files (Original)'!$D:$D,MATCH(1,($A2='Files (Original)'!$B:$B)*(_xlfn.NUMBERVALUE(H$1)='Files (Original)'!$C:$C),0)),"Missing")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4DAFC2A3-55D0-4A0A-8861-0AB5BF5FBA0D}" name="2020" dataDxfId="4">
+    <tableColumn id="9" xr3:uid="{4DAFC2A3-55D0-4A0A-8861-0AB5BF5FBA0D}" name="2020" dataDxfId="2">
       <calculatedColumnFormula array="1">IFERROR(INDEX('Files (Original)'!$D:$D,MATCH(1,($A2='Files (Original)'!$B:$B)*(_xlfn.NUMBERVALUE(I$1)='Files (Original)'!$C:$C),0)),"Missing")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F540DF46-6431-4312-92B2-096E64EDDA7A}" name="2021" dataDxfId="3">
+    <tableColumn id="10" xr3:uid="{F540DF46-6431-4312-92B2-096E64EDDA7A}" name="2021" dataDxfId="1">
       <calculatedColumnFormula array="1">IFERROR(INDEX('Files (Original)'!$D:$D,MATCH(1,($A2='Files (Original)'!$B:$B)*(_xlfn.NUMBERVALUE(J$1)='Files (Original)'!$C:$C),0)),"Missing")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{9A2EC175-5A3A-410C-B769-83323FE04F1D}" name="Reference Link" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{9A2EC175-5A3A-410C-B769-83323FE04F1D}" name="Reference Link" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2720,8 +2723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95844CC3-1EA9-4C4A-996F-0B8C6C506C2C}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4060,10 +4063,10 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="D2:J31">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"AR"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"Missing"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7053,10 +7056,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCCF928-8895-4AB9-B900-2E463F961084}">
-  <dimension ref="A1:B207"/>
+  <dimension ref="A1:E206"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="G89" sqref="G89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7064,1663 +7067,3510 @@
     <col min="1" max="1" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B1" t="s">
         <v>564</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>315</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D2">
+        <v>2015</v>
+      </c>
+      <c r="E2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>316</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D3">
+        <v>2016</v>
+      </c>
+      <c r="E3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>317</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D4">
+        <v>2017</v>
+      </c>
+      <c r="E4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>318</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5">
+        <v>2018</v>
+      </c>
+      <c r="E5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>319</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>209</v>
+      </c>
+      <c r="D6">
+        <v>2019</v>
+      </c>
+      <c r="E6" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>320</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7">
+        <v>2020</v>
+      </c>
+      <c r="E7" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>321</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>209</v>
+      </c>
+      <c r="D8">
+        <v>2021</v>
+      </c>
+      <c r="E8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>322</v>
       </c>
       <c r="B9" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>520</v>
+      </c>
+      <c r="C9" t="s">
+        <v>203</v>
+      </c>
+      <c r="D9">
+        <v>2015</v>
+      </c>
+      <c r="E9" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>323</v>
       </c>
       <c r="B10" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>521</v>
+      </c>
+      <c r="C10" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10">
+        <v>2016</v>
+      </c>
+      <c r="E10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>324</v>
       </c>
       <c r="B11" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>522</v>
+      </c>
+      <c r="C11" t="s">
+        <v>203</v>
+      </c>
+      <c r="D11">
+        <v>2017</v>
+      </c>
+      <c r="E11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>325</v>
       </c>
       <c r="B12" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>523</v>
+      </c>
+      <c r="C12" t="s">
+        <v>203</v>
+      </c>
+      <c r="D12">
+        <v>2018</v>
+      </c>
+      <c r="E12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>326</v>
       </c>
       <c r="B13" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>524</v>
+      </c>
+      <c r="C13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D13">
+        <v>2019</v>
+      </c>
+      <c r="E13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>327</v>
       </c>
       <c r="B14" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+        <v>525</v>
+      </c>
+      <c r="C14" t="s">
+        <v>203</v>
+      </c>
+      <c r="D14">
+        <v>2020</v>
+      </c>
+      <c r="E14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>328</v>
       </c>
       <c r="B15" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+        <v>526</v>
+      </c>
+      <c r="C15" t="s">
+        <v>203</v>
+      </c>
+      <c r="D15">
+        <v>2021</v>
+      </c>
+      <c r="E15" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>329</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>215</v>
+      </c>
+      <c r="D16">
+        <v>2015</v>
+      </c>
+      <c r="E16" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>330</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>215</v>
+      </c>
+      <c r="D17">
+        <v>2016</v>
+      </c>
+      <c r="E17" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>331</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>215</v>
+      </c>
+      <c r="D18">
+        <v>2017</v>
+      </c>
+      <c r="E18" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>332</v>
       </c>
       <c r="B19" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>215</v>
+      </c>
+      <c r="D19">
+        <v>2018</v>
+      </c>
+      <c r="E19" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>333</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>215</v>
+      </c>
+      <c r="D20">
+        <v>2019</v>
+      </c>
+      <c r="E20" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>334</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>215</v>
+      </c>
+      <c r="D21">
+        <v>2020</v>
+      </c>
+      <c r="E21" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>335</v>
       </c>
       <c r="B22" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>215</v>
+      </c>
+      <c r="D22">
+        <v>2021</v>
+      </c>
+      <c r="E22" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>336</v>
       </c>
       <c r="B23" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>227</v>
+      </c>
+      <c r="D23">
+        <v>2015</v>
+      </c>
+      <c r="E23" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>337</v>
       </c>
       <c r="B24" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>227</v>
+      </c>
+      <c r="D24">
+        <v>2016</v>
+      </c>
+      <c r="E24" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>338</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>227</v>
+      </c>
+      <c r="D25">
+        <v>2017</v>
+      </c>
+      <c r="E25" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>339</v>
       </c>
       <c r="B26" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D26">
+        <v>2018</v>
+      </c>
+      <c r="E26" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>340</v>
       </c>
       <c r="B27" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>227</v>
+      </c>
+      <c r="D27">
+        <v>2019</v>
+      </c>
+      <c r="E27" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>341</v>
       </c>
       <c r="B28" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>227</v>
+      </c>
+      <c r="D28">
+        <v>2020</v>
+      </c>
+      <c r="E28" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>342</v>
       </c>
       <c r="B29" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>227</v>
+      </c>
+      <c r="D29">
+        <v>2021</v>
+      </c>
+      <c r="E29" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>343</v>
       </c>
       <c r="B30" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>193</v>
+      </c>
+      <c r="D30">
+        <v>2015</v>
+      </c>
+      <c r="E30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>344</v>
       </c>
       <c r="B31" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>193</v>
+      </c>
+      <c r="D31">
+        <v>2016</v>
+      </c>
+      <c r="E31" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>345</v>
       </c>
       <c r="B32" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>193</v>
+      </c>
+      <c r="D32">
+        <v>2017</v>
+      </c>
+      <c r="E32" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>346</v>
       </c>
       <c r="B33" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>193</v>
+      </c>
+      <c r="D33">
+        <v>2018</v>
+      </c>
+      <c r="E33" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>347</v>
       </c>
       <c r="B34" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>193</v>
+      </c>
+      <c r="D34">
+        <v>2019</v>
+      </c>
+      <c r="E34" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>348</v>
       </c>
       <c r="B35" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>193</v>
+      </c>
+      <c r="D35">
+        <v>2020</v>
+      </c>
+      <c r="E35" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>349</v>
       </c>
       <c r="B36" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>193</v>
+      </c>
+      <c r="D36">
+        <v>2021</v>
+      </c>
+      <c r="E36" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>350</v>
       </c>
       <c r="B37" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+        <v>527</v>
+      </c>
+      <c r="C37" t="s">
+        <v>243</v>
+      </c>
+      <c r="D37">
+        <v>2015</v>
+      </c>
+      <c r="E37" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>351</v>
       </c>
       <c r="B38" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+        <v>528</v>
+      </c>
+      <c r="C38" t="s">
+        <v>243</v>
+      </c>
+      <c r="D38">
+        <v>2016</v>
+      </c>
+      <c r="E38" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>352</v>
       </c>
       <c r="B39" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+        <v>529</v>
+      </c>
+      <c r="C39" t="s">
+        <v>243</v>
+      </c>
+      <c r="D39">
+        <v>2017</v>
+      </c>
+      <c r="E39" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>353</v>
       </c>
       <c r="B40" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+        <v>530</v>
+      </c>
+      <c r="C40" t="s">
+        <v>243</v>
+      </c>
+      <c r="D40">
+        <v>2018</v>
+      </c>
+      <c r="E40" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>354</v>
       </c>
       <c r="B41" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+        <v>531</v>
+      </c>
+      <c r="C41" t="s">
+        <v>243</v>
+      </c>
+      <c r="D41">
+        <v>2019</v>
+      </c>
+      <c r="E41" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>355</v>
       </c>
       <c r="B42" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+        <v>532</v>
+      </c>
+      <c r="C42" t="s">
+        <v>243</v>
+      </c>
+      <c r="D42">
+        <v>2020</v>
+      </c>
+      <c r="E42" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>356</v>
       </c>
       <c r="B43" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+        <v>533</v>
+      </c>
+      <c r="C43" t="s">
+        <v>243</v>
+      </c>
+      <c r="D43">
+        <v>2021</v>
+      </c>
+      <c r="E43" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>357</v>
       </c>
       <c r="B44" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>197</v>
+      </c>
+      <c r="D44">
+        <v>2015</v>
+      </c>
+      <c r="E44" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>358</v>
       </c>
       <c r="B45" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>197</v>
+      </c>
+      <c r="D45">
+        <v>2016</v>
+      </c>
+      <c r="E45" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>359</v>
       </c>
       <c r="B46" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>197</v>
+      </c>
+      <c r="D46">
+        <v>2017</v>
+      </c>
+      <c r="E46" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>360</v>
       </c>
       <c r="B47" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>197</v>
+      </c>
+      <c r="D47">
+        <v>2018</v>
+      </c>
+      <c r="E47" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>361</v>
       </c>
       <c r="B48" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>197</v>
+      </c>
+      <c r="D48">
+        <v>2019</v>
+      </c>
+      <c r="E48" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>362</v>
       </c>
       <c r="B49" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>197</v>
+      </c>
+      <c r="D49">
+        <v>2020</v>
+      </c>
+      <c r="E49" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>363</v>
       </c>
       <c r="B50" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>197</v>
+      </c>
+      <c r="D50">
+        <v>2021</v>
+      </c>
+      <c r="E50" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>364</v>
       </c>
       <c r="B51" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>241</v>
+      </c>
+      <c r="D51">
+        <v>2017</v>
+      </c>
+      <c r="E51" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>365</v>
       </c>
       <c r="B52" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>241</v>
+      </c>
+      <c r="D52">
+        <v>2018</v>
+      </c>
+      <c r="E52" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>366</v>
       </c>
       <c r="B53" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>241</v>
+      </c>
+      <c r="D53">
+        <v>2019</v>
+      </c>
+      <c r="E53" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>367</v>
       </c>
       <c r="B54" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>241</v>
+      </c>
+      <c r="D54">
+        <v>2020</v>
+      </c>
+      <c r="E54" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>368</v>
       </c>
       <c r="B55" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>241</v>
+      </c>
+      <c r="D55">
+        <v>2021</v>
+      </c>
+      <c r="E55" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>369</v>
       </c>
       <c r="B56" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>237</v>
+      </c>
+      <c r="D56">
+        <v>2015</v>
+      </c>
+      <c r="E56" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>370</v>
       </c>
       <c r="B57" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>237</v>
+      </c>
+      <c r="D57">
+        <v>2016</v>
+      </c>
+      <c r="E57" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>371</v>
       </c>
       <c r="B58" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>237</v>
+      </c>
+      <c r="D58">
+        <v>2017</v>
+      </c>
+      <c r="E58" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>372</v>
       </c>
       <c r="B59" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>237</v>
+      </c>
+      <c r="D59">
+        <v>2018</v>
+      </c>
+      <c r="E59" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>373</v>
       </c>
       <c r="B60" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
+        <v>237</v>
+      </c>
+      <c r="D60">
+        <v>2019</v>
+      </c>
+      <c r="E60" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>374</v>
       </c>
       <c r="B61" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>237</v>
+      </c>
+      <c r="D61">
+        <v>2020</v>
+      </c>
+      <c r="E61" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>375</v>
       </c>
       <c r="B62" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>237</v>
+      </c>
+      <c r="D62">
+        <v>2021</v>
+      </c>
+      <c r="E62" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>376</v>
       </c>
       <c r="B63" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C63" t="s">
+        <v>247</v>
+      </c>
+      <c r="D63">
+        <v>2015</v>
+      </c>
+      <c r="E63" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>377</v>
       </c>
       <c r="B64" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
+        <v>247</v>
+      </c>
+      <c r="D64">
+        <v>2016</v>
+      </c>
+      <c r="E64" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>378</v>
       </c>
       <c r="B65" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
+        <v>247</v>
+      </c>
+      <c r="D65">
+        <v>2017</v>
+      </c>
+      <c r="E65" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>379</v>
       </c>
       <c r="B66" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>247</v>
+      </c>
+      <c r="D66">
+        <v>2018</v>
+      </c>
+      <c r="E66" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>380</v>
       </c>
       <c r="B67" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>247</v>
+      </c>
+      <c r="D67">
+        <v>2019</v>
+      </c>
+      <c r="E67" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>381</v>
       </c>
       <c r="B68" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C68" t="s">
+        <v>247</v>
+      </c>
+      <c r="D68">
+        <v>2020</v>
+      </c>
+      <c r="E68" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>382</v>
       </c>
       <c r="B69" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C69" t="s">
+        <v>247</v>
+      </c>
+      <c r="D69">
+        <v>2021</v>
+      </c>
+      <c r="E69" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>383</v>
       </c>
       <c r="B70" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+        <v>534</v>
+      </c>
+      <c r="C70" t="s">
+        <v>249</v>
+      </c>
+      <c r="D70">
+        <v>2015</v>
+      </c>
+      <c r="E70" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>384</v>
       </c>
       <c r="B71" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+        <v>535</v>
+      </c>
+      <c r="C71" t="s">
+        <v>249</v>
+      </c>
+      <c r="D71">
+        <v>2016</v>
+      </c>
+      <c r="E71" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>385</v>
       </c>
       <c r="B72" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
+        <v>249</v>
+      </c>
+      <c r="D72">
+        <v>2017</v>
+      </c>
+      <c r="E72" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>386</v>
       </c>
       <c r="B73" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C73" t="s">
+        <v>249</v>
+      </c>
+      <c r="D73">
+        <v>2018</v>
+      </c>
+      <c r="E73" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>387</v>
       </c>
       <c r="B74" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C74" t="s">
+        <v>249</v>
+      </c>
+      <c r="D74">
+        <v>2019</v>
+      </c>
+      <c r="E74" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>388</v>
       </c>
       <c r="B75" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C75" t="s">
+        <v>249</v>
+      </c>
+      <c r="D75">
+        <v>2020</v>
+      </c>
+      <c r="E75" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>389</v>
       </c>
       <c r="B76" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C76" t="s">
+        <v>249</v>
+      </c>
+      <c r="D76">
+        <v>2021</v>
+      </c>
+      <c r="E76" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>390</v>
       </c>
       <c r="B77" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+        <v>536</v>
+      </c>
+      <c r="C77" t="s">
+        <v>251</v>
+      </c>
+      <c r="D77">
+        <v>2015</v>
+      </c>
+      <c r="E77" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>391</v>
       </c>
       <c r="B78" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+        <v>537</v>
+      </c>
+      <c r="C78" t="s">
+        <v>251</v>
+      </c>
+      <c r="D78">
+        <v>2016</v>
+      </c>
+      <c r="E78" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>392</v>
       </c>
       <c r="B79" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+        <v>538</v>
+      </c>
+      <c r="C79" t="s">
+        <v>251</v>
+      </c>
+      <c r="D79">
+        <v>2017</v>
+      </c>
+      <c r="E79" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>393</v>
       </c>
       <c r="B80" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+        <v>539</v>
+      </c>
+      <c r="C80" t="s">
+        <v>251</v>
+      </c>
+      <c r="D80">
+        <v>2018</v>
+      </c>
+      <c r="E80" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>394</v>
       </c>
       <c r="B81" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+        <v>540</v>
+      </c>
+      <c r="C81" t="s">
+        <v>251</v>
+      </c>
+      <c r="D81">
+        <v>2019</v>
+      </c>
+      <c r="E81" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>395</v>
       </c>
       <c r="B82" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C82" t="s">
+        <v>251</v>
+      </c>
+      <c r="D82">
+        <v>2020</v>
+      </c>
+      <c r="E82" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>396</v>
       </c>
       <c r="B83" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C83" t="s">
+        <v>251</v>
+      </c>
+      <c r="D83">
+        <v>2021</v>
+      </c>
+      <c r="E83" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>397</v>
       </c>
       <c r="B84" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C84" t="s">
+        <v>201</v>
+      </c>
+      <c r="D84">
+        <v>2015</v>
+      </c>
+      <c r="E84" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>398</v>
       </c>
       <c r="B85" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C85" t="s">
+        <v>201</v>
+      </c>
+      <c r="D85">
+        <v>2016</v>
+      </c>
+      <c r="E85" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>399</v>
       </c>
       <c r="B86" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C86" t="s">
+        <v>201</v>
+      </c>
+      <c r="D86">
+        <v>2017</v>
+      </c>
+      <c r="E86" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>400</v>
       </c>
       <c r="B87" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C87" t="s">
+        <v>201</v>
+      </c>
+      <c r="D87">
+        <v>2018</v>
+      </c>
+      <c r="E87" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>401</v>
       </c>
       <c r="B88" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C88" t="s">
+        <v>201</v>
+      </c>
+      <c r="D88">
+        <v>2019</v>
+      </c>
+      <c r="E88" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>402</v>
       </c>
       <c r="B89" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C89" t="s">
+        <v>201</v>
+      </c>
+      <c r="D89">
+        <v>2020</v>
+      </c>
+      <c r="E89" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>403</v>
       </c>
       <c r="B90" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D90">
+        <v>2015</v>
+      </c>
+      <c r="E90" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>404</v>
       </c>
       <c r="B91" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C91" t="s">
+        <v>225</v>
+      </c>
+      <c r="D91">
+        <v>2016</v>
+      </c>
+      <c r="E91" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>405</v>
       </c>
       <c r="B92" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C92" t="s">
+        <v>225</v>
+      </c>
+      <c r="D92">
+        <v>2017</v>
+      </c>
+      <c r="E92" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>406</v>
       </c>
       <c r="B93" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C93" t="s">
+        <v>225</v>
+      </c>
+      <c r="D93">
+        <v>2018</v>
+      </c>
+      <c r="E93" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>407</v>
       </c>
       <c r="B94" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C94" t="s">
+        <v>225</v>
+      </c>
+      <c r="D94">
+        <v>2019</v>
+      </c>
+      <c r="E94" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>408</v>
       </c>
       <c r="B95" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C95" t="s">
+        <v>225</v>
+      </c>
+      <c r="D95">
+        <v>2020</v>
+      </c>
+      <c r="E95" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>409</v>
       </c>
       <c r="B96" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C96" t="s">
+        <v>225</v>
+      </c>
+      <c r="D96">
+        <v>2021</v>
+      </c>
+      <c r="E96" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>410</v>
       </c>
       <c r="B97" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="C97" t="s">
+        <v>217</v>
+      </c>
+      <c r="D97">
+        <v>2015</v>
+      </c>
+      <c r="E97" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>411</v>
       </c>
       <c r="B98" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="C98" t="s">
+        <v>217</v>
+      </c>
+      <c r="D98">
+        <v>2016</v>
+      </c>
+      <c r="E98" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>412</v>
       </c>
       <c r="B99" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="C99" t="s">
+        <v>217</v>
+      </c>
+      <c r="D99">
+        <v>2017</v>
+      </c>
+      <c r="E99" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>413</v>
       </c>
       <c r="B100" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+      <c r="C100" t="s">
+        <v>217</v>
+      </c>
+      <c r="D100">
+        <v>2018</v>
+      </c>
+      <c r="E100" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>414</v>
       </c>
       <c r="B101" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="C101" t="s">
+        <v>217</v>
+      </c>
+      <c r="D101">
+        <v>2019</v>
+      </c>
+      <c r="E101" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>415</v>
       </c>
       <c r="B102" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+      <c r="C102" t="s">
+        <v>217</v>
+      </c>
+      <c r="D102">
+        <v>2020</v>
+      </c>
+      <c r="E102" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>416</v>
       </c>
       <c r="B103" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="C103" t="s">
+        <v>217</v>
+      </c>
+      <c r="D103">
+        <v>2021</v>
+      </c>
+      <c r="E103" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>417</v>
       </c>
       <c r="B104" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="C104" t="s">
+        <v>223</v>
+      </c>
+      <c r="D104">
+        <v>2015</v>
+      </c>
+      <c r="E104" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>418</v>
       </c>
       <c r="B105" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+      <c r="C105" t="s">
+        <v>223</v>
+      </c>
+      <c r="D105">
+        <v>2016</v>
+      </c>
+      <c r="E105" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>419</v>
       </c>
       <c r="B106" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+      <c r="C106" t="s">
+        <v>223</v>
+      </c>
+      <c r="D106">
+        <v>2017</v>
+      </c>
+      <c r="E106" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>420</v>
       </c>
       <c r="B107" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="C107" t="s">
+        <v>223</v>
+      </c>
+      <c r="D107">
+        <v>2018</v>
+      </c>
+      <c r="E107" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>421</v>
       </c>
       <c r="B108" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+      <c r="C108" t="s">
+        <v>223</v>
+      </c>
+      <c r="D108">
+        <v>2019</v>
+      </c>
+      <c r="E108" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>422</v>
       </c>
       <c r="B109" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="C109" t="s">
+        <v>223</v>
+      </c>
+      <c r="D109">
+        <v>2020</v>
+      </c>
+      <c r="E109" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>423</v>
       </c>
       <c r="B110" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="C110" t="s">
+        <v>223</v>
+      </c>
+      <c r="D110">
+        <v>2021</v>
+      </c>
+      <c r="E110" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>424</v>
       </c>
       <c r="B111" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+      <c r="C111" t="s">
+        <v>207</v>
+      </c>
+      <c r="D111">
+        <v>2015</v>
+      </c>
+      <c r="E111" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>425</v>
       </c>
       <c r="B112" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="C112" t="s">
+        <v>207</v>
+      </c>
+      <c r="D112">
+        <v>2016</v>
+      </c>
+      <c r="E112" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>426</v>
       </c>
       <c r="B113" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="C113" t="s">
+        <v>207</v>
+      </c>
+      <c r="D113">
+        <v>2017</v>
+      </c>
+      <c r="E113" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>427</v>
       </c>
       <c r="B114" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="C114" t="s">
+        <v>207</v>
+      </c>
+      <c r="D114">
+        <v>2018</v>
+      </c>
+      <c r="E114" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>428</v>
       </c>
       <c r="B115" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="C115" t="s">
+        <v>207</v>
+      </c>
+      <c r="D115">
+        <v>2019</v>
+      </c>
+      <c r="E115" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>429</v>
       </c>
       <c r="B116" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="C116" t="s">
+        <v>207</v>
+      </c>
+      <c r="D116">
+        <v>2020</v>
+      </c>
+      <c r="E116" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>430</v>
       </c>
       <c r="B117" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="C117" t="s">
+        <v>207</v>
+      </c>
+      <c r="D117">
+        <v>2021</v>
+      </c>
+      <c r="E117" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>431</v>
       </c>
       <c r="B118" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="C118" t="s">
+        <v>211</v>
+      </c>
+      <c r="D118">
+        <v>2015</v>
+      </c>
+      <c r="E118" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>432</v>
       </c>
       <c r="B119" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+        <v>541</v>
+      </c>
+      <c r="C119" t="s">
+        <v>211</v>
+      </c>
+      <c r="D119">
+        <v>2016</v>
+      </c>
+      <c r="E119" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>433</v>
       </c>
       <c r="B120" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+      <c r="C120" t="s">
+        <v>211</v>
+      </c>
+      <c r="D120">
+        <v>2017</v>
+      </c>
+      <c r="E120" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>434</v>
       </c>
       <c r="B121" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="C121" t="s">
+        <v>211</v>
+      </c>
+      <c r="D121">
+        <v>2018</v>
+      </c>
+      <c r="E121" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>435</v>
       </c>
       <c r="B122" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="C122" t="s">
+        <v>211</v>
+      </c>
+      <c r="D122">
+        <v>2019</v>
+      </c>
+      <c r="E122" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>436</v>
       </c>
       <c r="B123" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="C123" t="s">
+        <v>211</v>
+      </c>
+      <c r="D123">
+        <v>2020</v>
+      </c>
+      <c r="E123" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>437</v>
       </c>
       <c r="B124" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="C124" t="s">
+        <v>211</v>
+      </c>
+      <c r="D124">
+        <v>2021</v>
+      </c>
+      <c r="E124" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>438</v>
       </c>
       <c r="B125" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+        <v>542</v>
+      </c>
+      <c r="C125" t="s">
+        <v>231</v>
+      </c>
+      <c r="D125">
+        <v>2015</v>
+      </c>
+      <c r="E125" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>439</v>
       </c>
       <c r="B126" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C126" t="s">
+        <v>231</v>
+      </c>
+      <c r="D126">
+        <v>2016</v>
+      </c>
+      <c r="E126" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>440</v>
       </c>
       <c r="B127" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+      <c r="C127" t="s">
+        <v>231</v>
+      </c>
+      <c r="D127">
+        <v>2017</v>
+      </c>
+      <c r="E127" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>441</v>
       </c>
       <c r="B128" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+      <c r="C128" t="s">
+        <v>231</v>
+      </c>
+      <c r="D128">
+        <v>2018</v>
+      </c>
+      <c r="E128" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>442</v>
       </c>
       <c r="B129" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+      <c r="C129" t="s">
+        <v>231</v>
+      </c>
+      <c r="D129">
+        <v>2019</v>
+      </c>
+      <c r="E129" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>443</v>
       </c>
       <c r="B130" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+      <c r="C130" t="s">
+        <v>231</v>
+      </c>
+      <c r="D130">
+        <v>2020</v>
+      </c>
+      <c r="E130" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>444</v>
       </c>
       <c r="B131" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+      <c r="C131" t="s">
+        <v>231</v>
+      </c>
+      <c r="D131">
+        <v>2021</v>
+      </c>
+      <c r="E131" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>445</v>
       </c>
       <c r="B132" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+        <v>544</v>
+      </c>
+      <c r="C132" t="s">
+        <v>229</v>
+      </c>
+      <c r="D132">
+        <v>2015</v>
+      </c>
+      <c r="E132" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>446</v>
       </c>
       <c r="B133" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C133" t="s">
+        <v>229</v>
+      </c>
+      <c r="D133">
+        <v>2016</v>
+      </c>
+      <c r="E133" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>447</v>
       </c>
       <c r="B134" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+      <c r="C134" t="s">
+        <v>229</v>
+      </c>
+      <c r="D134">
+        <v>2017</v>
+      </c>
+      <c r="E134" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>448</v>
       </c>
       <c r="B135" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="C135" t="s">
+        <v>229</v>
+      </c>
+      <c r="D135">
+        <v>2018</v>
+      </c>
+      <c r="E135" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>449</v>
       </c>
       <c r="B136" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="C136" t="s">
+        <v>229</v>
+      </c>
+      <c r="D136">
+        <v>2019</v>
+      </c>
+      <c r="E136" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>450</v>
       </c>
       <c r="B137" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="C137" t="s">
+        <v>229</v>
+      </c>
+      <c r="D137">
+        <v>2020</v>
+      </c>
+      <c r="E137" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>451</v>
       </c>
       <c r="B138" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+      <c r="C138" t="s">
+        <v>229</v>
+      </c>
+      <c r="D138">
+        <v>2021</v>
+      </c>
+      <c r="E138" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>452</v>
       </c>
       <c r="B139" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+      <c r="C139" t="s">
+        <v>245</v>
+      </c>
+      <c r="D139">
+        <v>2015</v>
+      </c>
+      <c r="E139" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>453</v>
       </c>
       <c r="B140" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+      <c r="C140" t="s">
+        <v>245</v>
+      </c>
+      <c r="D140">
+        <v>2016</v>
+      </c>
+      <c r="E140" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>454</v>
       </c>
       <c r="B141" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+      <c r="C141" t="s">
+        <v>245</v>
+      </c>
+      <c r="D141">
+        <v>2017</v>
+      </c>
+      <c r="E141" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>455</v>
       </c>
       <c r="B142" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+      <c r="C142" t="s">
+        <v>245</v>
+      </c>
+      <c r="D142">
+        <v>2018</v>
+      </c>
+      <c r="E142" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>456</v>
       </c>
       <c r="B143" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+      <c r="C143" t="s">
+        <v>245</v>
+      </c>
+      <c r="D143">
+        <v>2019</v>
+      </c>
+      <c r="E143" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>457</v>
       </c>
       <c r="B144" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+      <c r="C144" t="s">
+        <v>245</v>
+      </c>
+      <c r="D144">
+        <v>2020</v>
+      </c>
+      <c r="E144" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>458</v>
       </c>
       <c r="B145" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+      <c r="C145" t="s">
+        <v>245</v>
+      </c>
+      <c r="D145">
+        <v>2021</v>
+      </c>
+      <c r="E145" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>459</v>
       </c>
       <c r="B146" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+        <v>546</v>
+      </c>
+      <c r="C146" t="s">
+        <v>235</v>
+      </c>
+      <c r="D146">
+        <v>2015</v>
+      </c>
+      <c r="E146" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>460</v>
       </c>
       <c r="B147" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C147" t="s">
+        <v>235</v>
+      </c>
+      <c r="D147">
+        <v>2016</v>
+      </c>
+      <c r="E147" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>461</v>
       </c>
       <c r="B148" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C148" t="s">
+        <v>235</v>
+      </c>
+      <c r="D148">
+        <v>2017</v>
+      </c>
+      <c r="E148" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>462</v>
       </c>
       <c r="B149" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C149" t="s">
+        <v>235</v>
+      </c>
+      <c r="D149">
+        <v>2018</v>
+      </c>
+      <c r="E149" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>463</v>
       </c>
       <c r="B150" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C150" t="s">
+        <v>235</v>
+      </c>
+      <c r="D150">
+        <v>2019</v>
+      </c>
+      <c r="E150" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>464</v>
       </c>
       <c r="B151" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C151" t="s">
+        <v>235</v>
+      </c>
+      <c r="D151">
+        <v>2020</v>
+      </c>
+      <c r="E151" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>465</v>
       </c>
       <c r="B152" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C152" t="s">
+        <v>235</v>
+      </c>
+      <c r="D152">
+        <v>2021</v>
+      </c>
+      <c r="E152" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>466</v>
       </c>
       <c r="B153" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C153" t="s">
+        <v>239</v>
+      </c>
+      <c r="D153">
+        <v>2015</v>
+      </c>
+      <c r="E153" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>467</v>
       </c>
       <c r="B154" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+      <c r="C154" t="s">
+        <v>239</v>
+      </c>
+      <c r="D154">
+        <v>2016</v>
+      </c>
+      <c r="E154" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>468</v>
       </c>
       <c r="B155" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+      <c r="C155" t="s">
+        <v>239</v>
+      </c>
+      <c r="D155">
+        <v>2017</v>
+      </c>
+      <c r="E155" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>469</v>
       </c>
       <c r="B156" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+      <c r="C156" t="s">
+        <v>239</v>
+      </c>
+      <c r="D156">
+        <v>2018</v>
+      </c>
+      <c r="E156" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>470</v>
       </c>
       <c r="B157" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+      <c r="C157" t="s">
+        <v>239</v>
+      </c>
+      <c r="D157">
+        <v>2019</v>
+      </c>
+      <c r="E157" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>471</v>
       </c>
       <c r="B158" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="C158" t="s">
+        <v>239</v>
+      </c>
+      <c r="D158">
+        <v>2020</v>
+      </c>
+      <c r="E158" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>472</v>
       </c>
       <c r="B159" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+      <c r="C159" t="s">
+        <v>239</v>
+      </c>
+      <c r="D159">
+        <v>2021</v>
+      </c>
+      <c r="E159" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>473</v>
       </c>
       <c r="B160" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+      <c r="C160" t="s">
+        <v>199</v>
+      </c>
+      <c r="D160">
+        <v>2015</v>
+      </c>
+      <c r="E160" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>474</v>
       </c>
       <c r="B161" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="C161" t="s">
+        <v>199</v>
+      </c>
+      <c r="D161">
+        <v>2016</v>
+      </c>
+      <c r="E161" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>475</v>
       </c>
       <c r="B162" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+      <c r="C162" t="s">
+        <v>199</v>
+      </c>
+      <c r="D162">
+        <v>2017</v>
+      </c>
+      <c r="E162" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>476</v>
       </c>
       <c r="B163" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+      <c r="C163" t="s">
+        <v>199</v>
+      </c>
+      <c r="D163">
+        <v>2018</v>
+      </c>
+      <c r="E163" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>477</v>
       </c>
       <c r="B164" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+      <c r="C164" t="s">
+        <v>199</v>
+      </c>
+      <c r="D164">
+        <v>2019</v>
+      </c>
+      <c r="E164" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>478</v>
       </c>
       <c r="B165" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+      <c r="C165" t="s">
+        <v>199</v>
+      </c>
+      <c r="D165">
+        <v>2020</v>
+      </c>
+      <c r="E165" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>479</v>
       </c>
       <c r="B166" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+      <c r="C166" t="s">
+        <v>199</v>
+      </c>
+      <c r="D166">
+        <v>2021</v>
+      </c>
+      <c r="E166" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>480</v>
       </c>
       <c r="B167" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+      <c r="C167" t="s">
+        <v>219</v>
+      </c>
+      <c r="D167">
+        <v>2015</v>
+      </c>
+      <c r="E167" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>481</v>
       </c>
       <c r="B168" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+      <c r="C168" t="s">
+        <v>219</v>
+      </c>
+      <c r="D168">
+        <v>2016</v>
+      </c>
+      <c r="E168" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>482</v>
       </c>
       <c r="B169" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+      <c r="C169" t="s">
+        <v>219</v>
+      </c>
+      <c r="D169">
+        <v>2017</v>
+      </c>
+      <c r="E169" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>483</v>
       </c>
       <c r="B170" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+      <c r="C170" t="s">
+        <v>219</v>
+      </c>
+      <c r="D170">
+        <v>2018</v>
+      </c>
+      <c r="E170" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>484</v>
       </c>
       <c r="B171" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+      <c r="C171" t="s">
+        <v>219</v>
+      </c>
+      <c r="D171">
+        <v>2019</v>
+      </c>
+      <c r="E171" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>485</v>
       </c>
       <c r="B172" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+      <c r="C172" t="s">
+        <v>219</v>
+      </c>
+      <c r="D172">
+        <v>2020</v>
+      </c>
+      <c r="E172" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>486</v>
       </c>
       <c r="B173" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+      <c r="C173" t="s">
+        <v>219</v>
+      </c>
+      <c r="D173">
+        <v>2021</v>
+      </c>
+      <c r="E173" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>487</v>
       </c>
       <c r="B174" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+        <v>554</v>
+      </c>
+      <c r="C174" t="s">
+        <v>205</v>
+      </c>
+      <c r="D174">
+        <v>2015</v>
+      </c>
+      <c r="E174" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>488</v>
       </c>
       <c r="B175" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C175" t="s">
+        <v>205</v>
+      </c>
+      <c r="D175">
+        <v>2016</v>
+      </c>
+      <c r="E175" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>489</v>
       </c>
       <c r="B176" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C176" t="s">
+        <v>205</v>
+      </c>
+      <c r="D176">
+        <v>2017</v>
+      </c>
+      <c r="E176" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>490</v>
       </c>
       <c r="B177" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C177" t="s">
+        <v>205</v>
+      </c>
+      <c r="D177">
+        <v>2018</v>
+      </c>
+      <c r="E177" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>491</v>
       </c>
       <c r="B178" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C178" t="s">
+        <v>205</v>
+      </c>
+      <c r="D178">
+        <v>2019</v>
+      </c>
+      <c r="E178" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>492</v>
       </c>
       <c r="B179" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+      <c r="C179" t="s">
+        <v>205</v>
+      </c>
+      <c r="D179">
+        <v>2020</v>
+      </c>
+      <c r="E179" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>493</v>
       </c>
       <c r="B180" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+      <c r="C180" t="s">
+        <v>205</v>
+      </c>
+      <c r="D180">
+        <v>2021</v>
+      </c>
+      <c r="E180" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>494</v>
       </c>
       <c r="B181" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+      <c r="C181" t="s">
+        <v>233</v>
+      </c>
+      <c r="D181">
+        <v>2015</v>
+      </c>
+      <c r="E181" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>495</v>
       </c>
       <c r="B182" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+      <c r="C182" t="s">
+        <v>233</v>
+      </c>
+      <c r="D182">
+        <v>2016</v>
+      </c>
+      <c r="E182" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>496</v>
       </c>
       <c r="B183" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+      <c r="C183" t="s">
+        <v>233</v>
+      </c>
+      <c r="D183">
+        <v>2017</v>
+      </c>
+      <c r="E183" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>497</v>
       </c>
       <c r="B184" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+      <c r="C184" t="s">
+        <v>233</v>
+      </c>
+      <c r="D184">
+        <v>2018</v>
+      </c>
+      <c r="E184" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>498</v>
       </c>
       <c r="B185" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+      <c r="C185" t="s">
+        <v>233</v>
+      </c>
+      <c r="D185">
+        <v>2019</v>
+      </c>
+      <c r="E185" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>499</v>
       </c>
       <c r="B186" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+      <c r="C186" t="s">
+        <v>233</v>
+      </c>
+      <c r="D186">
+        <v>2020</v>
+      </c>
+      <c r="E186" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>500</v>
       </c>
       <c r="B187" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+        <v>285</v>
+      </c>
+      <c r="C187" t="s">
+        <v>233</v>
+      </c>
+      <c r="D187">
+        <v>2021</v>
+      </c>
+      <c r="E187" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>501</v>
       </c>
       <c r="B188" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+      <c r="C188" t="s">
+        <v>195</v>
+      </c>
+      <c r="D188">
+        <v>2017</v>
+      </c>
+      <c r="E188" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>502</v>
       </c>
       <c r="B189" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+      <c r="C189" t="s">
+        <v>195</v>
+      </c>
+      <c r="D189">
+        <v>2018</v>
+      </c>
+      <c r="E189" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>503</v>
       </c>
       <c r="B190" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+      <c r="C190" t="s">
+        <v>195</v>
+      </c>
+      <c r="D190">
+        <v>2019</v>
+      </c>
+      <c r="E190" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>504</v>
       </c>
       <c r="B191" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+      <c r="C191" t="s">
+        <v>195</v>
+      </c>
+      <c r="D191">
+        <v>2020</v>
+      </c>
+      <c r="E191" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>505</v>
       </c>
       <c r="B192" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+      <c r="C192" t="s">
+        <v>195</v>
+      </c>
+      <c r="D192">
+        <v>2021</v>
+      </c>
+      <c r="E192" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>506</v>
       </c>
       <c r="B193" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+      <c r="C193" t="s">
+        <v>221</v>
+      </c>
+      <c r="D193">
+        <v>2015</v>
+      </c>
+      <c r="E193" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>507</v>
       </c>
       <c r="B194" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+      <c r="C194" t="s">
+        <v>221</v>
+      </c>
+      <c r="D194">
+        <v>2016</v>
+      </c>
+      <c r="E194" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>508</v>
       </c>
       <c r="B195" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+      <c r="C195" t="s">
+        <v>221</v>
+      </c>
+      <c r="D195">
+        <v>2017</v>
+      </c>
+      <c r="E195" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>509</v>
       </c>
       <c r="B196" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="C196" t="s">
+        <v>221</v>
+      </c>
+      <c r="D196">
+        <v>2018</v>
+      </c>
+      <c r="E196" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>510</v>
       </c>
       <c r="B197" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="C197" t="s">
+        <v>221</v>
+      </c>
+      <c r="D197">
+        <v>2019</v>
+      </c>
+      <c r="E197" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>511</v>
       </c>
       <c r="B198" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+      <c r="C198" t="s">
+        <v>221</v>
+      </c>
+      <c r="D198">
+        <v>2020</v>
+      </c>
+      <c r="E198" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>512</v>
       </c>
       <c r="B199" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+        <v>283</v>
+      </c>
+      <c r="C199" t="s">
+        <v>221</v>
+      </c>
+      <c r="D199">
+        <v>2021</v>
+      </c>
+      <c r="E199" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>513</v>
       </c>
       <c r="B200" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+        <v>559</v>
+      </c>
+      <c r="C200" t="s">
+        <v>213</v>
+      </c>
+      <c r="D200">
+        <v>2015</v>
+      </c>
+      <c r="E200" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>514</v>
       </c>
       <c r="B201" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C201" t="s">
+        <v>213</v>
+      </c>
+      <c r="D201">
+        <v>2016</v>
+      </c>
+      <c r="E201" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>515</v>
       </c>
       <c r="B202" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C202" t="s">
+        <v>213</v>
+      </c>
+      <c r="D202">
+        <v>2017</v>
+      </c>
+      <c r="E202" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>516</v>
       </c>
       <c r="B203" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C203" t="s">
+        <v>213</v>
+      </c>
+      <c r="D203">
+        <v>2018</v>
+      </c>
+      <c r="E203" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>517</v>
       </c>
       <c r="B204" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+      <c r="C204" t="s">
+        <v>213</v>
+      </c>
+      <c r="D204">
+        <v>2019</v>
+      </c>
+      <c r="E204" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>518</v>
       </c>
       <c r="B205" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+      <c r="C205" t="s">
+        <v>213</v>
+      </c>
+      <c r="D205">
+        <v>2020</v>
+      </c>
+      <c r="E205" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>519</v>
       </c>
       <c r="B206" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A207" t="s">
-        <v>520</v>
-      </c>
-      <c r="B207" t="s">
         <v>300</v>
       </c>
+      <c r="C206" t="s">
+        <v>213</v>
+      </c>
+      <c r="D206">
+        <v>2021</v>
+      </c>
+      <c r="E206" t="s">
+        <v>258</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E206" xr:uid="{1CCCF928-8895-4AB9-B900-2E463F961084}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more methodology + update to list of reports
</commit_message>
<xml_diff>
--- a/List of Companies and Sustainability Reports.xlsx
+++ b/List of Companies and Sustainability Reports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy Chia\Documents\GitHub\NLP-SustainabilityReports-FinancialPerformance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2241BF06-108E-4E3B-96E2-E2BF5D2E509A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A38917-3AF8-429F-BB82-CB8D98E4C09A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Companies" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Files (New)" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Files (New)'!$A$1:$E$206</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Files (New)'!$A$1:$E$207</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="570">
   <si>
     <t>ASCENDAS REAL ESTATE INV TRUST_2015_SUS.pdf</t>
   </si>
@@ -1771,6 +1771,9 @@
   </si>
   <si>
     <t>KEPPEL CORPORATION LIMITED_2021_SUS.pdf</t>
+  </si>
+  <si>
+    <t>C:\Users\Jeremy Chia\Documents\GitHub\NLP-SustainabilityReports-FinancialPerformance\Sustainability Reports or Annual Reports\KEPPEL CORPORATION LIMITED_2021_SUS.pdf</t>
   </si>
 </sst>
 </file>
@@ -4254,8 +4257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95844CC3-1EA9-4C4A-996F-0B8C6C506C2C}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5657,8 +5660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D207"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="A125" sqref="A125"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90:D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9573,10 +9576,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCCF928-8895-4AB9-B900-2E463F961084}">
-  <dimension ref="A1:E206"/>
+  <dimension ref="A1:E207"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
+      <selection sqref="A1:E207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11099,16 +11102,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>400</v>
+        <v>569</v>
       </c>
       <c r="B90" t="s">
-        <v>76</v>
+        <v>568</v>
       </c>
       <c r="C90" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="D90">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E90" t="s">
         <v>255</v>
@@ -11116,16 +11119,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B91" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C91" t="s">
         <v>222</v>
       </c>
       <c r="D91">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E91" t="s">
         <v>255</v>
@@ -11133,16 +11136,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B92" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C92" t="s">
         <v>222</v>
       </c>
       <c r="D92">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E92" t="s">
         <v>255</v>
@@ -11150,16 +11153,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B93" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C93" t="s">
         <v>222</v>
       </c>
       <c r="D93">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E93" t="s">
         <v>255</v>
@@ -11167,16 +11170,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B94" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C94" t="s">
         <v>222</v>
       </c>
       <c r="D94">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E94" t="s">
         <v>255</v>
@@ -11184,16 +11187,16 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B95" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C95" t="s">
         <v>222</v>
       </c>
       <c r="D95">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E95" t="s">
         <v>255</v>
@@ -11201,16 +11204,16 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B96" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C96" t="s">
         <v>222</v>
       </c>
       <c r="D96">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E96" t="s">
         <v>255</v>
@@ -11218,16 +11221,16 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B97" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C97" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="D97">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E97" t="s">
         <v>255</v>
@@ -11235,16 +11238,16 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B98" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C98" t="s">
         <v>214</v>
       </c>
       <c r="D98">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E98" t="s">
         <v>255</v>
@@ -11252,16 +11255,16 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B99" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C99" t="s">
         <v>214</v>
       </c>
       <c r="D99">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E99" t="s">
         <v>255</v>
@@ -11269,16 +11272,16 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B100" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C100" t="s">
         <v>214</v>
       </c>
       <c r="D100">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E100" t="s">
         <v>255</v>
@@ -11286,16 +11289,16 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B101" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C101" t="s">
         <v>214</v>
       </c>
       <c r="D101">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E101" t="s">
         <v>255</v>
@@ -11303,16 +11306,16 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B102" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C102" t="s">
         <v>214</v>
       </c>
       <c r="D102">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E102" t="s">
         <v>255</v>
@@ -11320,16 +11323,16 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B103" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C103" t="s">
         <v>214</v>
       </c>
       <c r="D103">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E103" t="s">
         <v>255</v>
@@ -11337,16 +11340,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B104" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C104" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D104">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E104" t="s">
         <v>255</v>
@@ -11354,16 +11357,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B105" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C105" t="s">
         <v>220</v>
       </c>
       <c r="D105">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E105" t="s">
         <v>255</v>
@@ -11371,16 +11374,16 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B106" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C106" t="s">
         <v>220</v>
       </c>
       <c r="D106">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E106" t="s">
         <v>255</v>
@@ -11388,16 +11391,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B107" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C107" t="s">
         <v>220</v>
       </c>
       <c r="D107">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E107" t="s">
         <v>255</v>
@@ -11405,16 +11408,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B108" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C108" t="s">
         <v>220</v>
       </c>
       <c r="D108">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E108" t="s">
         <v>255</v>
@@ -11422,16 +11425,16 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B109" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C109" t="s">
         <v>220</v>
       </c>
       <c r="D109">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E109" t="s">
         <v>255</v>
@@ -11439,16 +11442,16 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B110" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C110" t="s">
         <v>220</v>
       </c>
       <c r="D110">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E110" t="s">
         <v>255</v>
@@ -11456,16 +11459,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B111" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C111" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
       <c r="D111">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E111" t="s">
         <v>255</v>
@@ -11473,16 +11476,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B112" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C112" t="s">
         <v>204</v>
       </c>
       <c r="D112">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E112" t="s">
         <v>255</v>
@@ -11490,16 +11493,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B113" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C113" t="s">
         <v>204</v>
       </c>
       <c r="D113">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E113" t="s">
         <v>255</v>
@@ -11507,16 +11510,16 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B114" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C114" t="s">
         <v>204</v>
       </c>
       <c r="D114">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E114" t="s">
         <v>255</v>
@@ -11524,16 +11527,16 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B115" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C115" t="s">
         <v>204</v>
       </c>
       <c r="D115">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E115" t="s">
         <v>255</v>
@@ -11541,16 +11544,16 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B116" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C116" t="s">
         <v>204</v>
       </c>
       <c r="D116">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E116" t="s">
         <v>255</v>
@@ -11558,16 +11561,16 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B117" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C117" t="s">
         <v>204</v>
       </c>
       <c r="D117">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E117" t="s">
         <v>255</v>
@@ -11575,16 +11578,16 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B118" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C118" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D118">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E118" t="s">
         <v>255</v>
@@ -11592,16 +11595,16 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B119" t="s">
-        <v>538</v>
+        <v>104</v>
       </c>
       <c r="C119" t="s">
         <v>208</v>
       </c>
       <c r="D119">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E119" t="s">
         <v>255</v>
@@ -11609,16 +11612,16 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B120" t="s">
-        <v>106</v>
+        <v>538</v>
       </c>
       <c r="C120" t="s">
         <v>208</v>
       </c>
       <c r="D120">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E120" t="s">
         <v>255</v>
@@ -11626,16 +11629,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B121" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C121" t="s">
         <v>208</v>
       </c>
       <c r="D121">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E121" t="s">
         <v>255</v>
@@ -11643,16 +11646,16 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B122" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C122" t="s">
         <v>208</v>
       </c>
       <c r="D122">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E122" t="s">
         <v>255</v>
@@ -11660,16 +11663,16 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B123" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C123" t="s">
         <v>208</v>
       </c>
       <c r="D123">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E123" t="s">
         <v>255</v>
@@ -11677,16 +11680,16 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B124" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C124" t="s">
         <v>208</v>
       </c>
       <c r="D124">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E124" t="s">
         <v>255</v>
@@ -11694,16 +11697,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B125" t="s">
-        <v>539</v>
+        <v>110</v>
       </c>
       <c r="C125" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="D125">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E125" t="s">
         <v>255</v>
@@ -11711,16 +11714,16 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B126" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C126" t="s">
         <v>228</v>
       </c>
       <c r="D126">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E126" t="s">
         <v>255</v>
@@ -11728,16 +11731,16 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B127" t="s">
-        <v>113</v>
+        <v>540</v>
       </c>
       <c r="C127" t="s">
         <v>228</v>
       </c>
       <c r="D127">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E127" t="s">
         <v>255</v>
@@ -11745,16 +11748,16 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B128" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C128" t="s">
         <v>228</v>
       </c>
       <c r="D128">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E128" t="s">
         <v>255</v>
@@ -11762,16 +11765,16 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B129" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C129" t="s">
         <v>228</v>
       </c>
       <c r="D129">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E129" t="s">
         <v>255</v>
@@ -11779,16 +11782,16 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B130" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C130" t="s">
         <v>228</v>
       </c>
       <c r="D130">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E130" t="s">
         <v>255</v>
@@ -11796,16 +11799,16 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B131" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C131" t="s">
         <v>228</v>
       </c>
       <c r="D131">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E131" t="s">
         <v>255</v>
@@ -11813,16 +11816,16 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B132" t="s">
-        <v>541</v>
+        <v>117</v>
       </c>
       <c r="C132" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D132">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E132" t="s">
         <v>255</v>
@@ -11830,16 +11833,16 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B133" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C133" t="s">
         <v>226</v>
       </c>
       <c r="D133">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E133" t="s">
         <v>255</v>
@@ -11847,16 +11850,16 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B134" t="s">
-        <v>120</v>
+        <v>542</v>
       </c>
       <c r="C134" t="s">
         <v>226</v>
       </c>
       <c r="D134">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E134" t="s">
         <v>255</v>
@@ -11864,16 +11867,16 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B135" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C135" t="s">
         <v>226</v>
       </c>
       <c r="D135">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E135" t="s">
         <v>255</v>
@@ -11881,16 +11884,16 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B136" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C136" t="s">
         <v>226</v>
       </c>
       <c r="D136">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E136" t="s">
         <v>255</v>
@@ -11898,16 +11901,16 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B137" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C137" t="s">
         <v>226</v>
       </c>
       <c r="D137">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E137" t="s">
         <v>255</v>
@@ -11915,16 +11918,16 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B138" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C138" t="s">
         <v>226</v>
       </c>
       <c r="D138">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E138" t="s">
         <v>255</v>
@@ -11932,16 +11935,16 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B139" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C139" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="D139">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E139" t="s">
         <v>255</v>
@@ -11949,16 +11952,16 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B140" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C140" t="s">
         <v>242</v>
       </c>
       <c r="D140">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E140" t="s">
         <v>255</v>
@@ -11966,16 +11969,16 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B141" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C141" t="s">
         <v>242</v>
       </c>
       <c r="D141">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E141" t="s">
         <v>255</v>
@@ -11983,16 +11986,16 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B142" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C142" t="s">
         <v>242</v>
       </c>
       <c r="D142">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E142" t="s">
         <v>255</v>
@@ -12000,16 +12003,16 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B143" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C143" t="s">
         <v>242</v>
       </c>
       <c r="D143">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E143" t="s">
         <v>255</v>
@@ -12017,16 +12020,16 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B144" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C144" t="s">
         <v>242</v>
       </c>
       <c r="D144">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E144" t="s">
         <v>255</v>
@@ -12034,16 +12037,16 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B145" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C145" t="s">
         <v>242</v>
       </c>
       <c r="D145">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E145" t="s">
         <v>255</v>
@@ -12051,16 +12054,16 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B146" t="s">
-        <v>543</v>
+        <v>131</v>
       </c>
       <c r="C146" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="D146">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E146" t="s">
         <v>255</v>
@@ -12068,16 +12071,16 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B147" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C147" t="s">
         <v>232</v>
       </c>
       <c r="D147">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E147" t="s">
         <v>255</v>
@@ -12085,16 +12088,16 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B148" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C148" t="s">
         <v>232</v>
       </c>
       <c r="D148">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E148" t="s">
         <v>255</v>
@@ -12102,16 +12105,16 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B149" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C149" t="s">
         <v>232</v>
       </c>
       <c r="D149">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E149" t="s">
         <v>255</v>
@@ -12119,16 +12122,16 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B150" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C150" t="s">
         <v>232</v>
       </c>
       <c r="D150">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E150" t="s">
         <v>255</v>
@@ -12136,16 +12139,16 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B151" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C151" t="s">
         <v>232</v>
       </c>
       <c r="D151">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E151" t="s">
         <v>255</v>
@@ -12153,16 +12156,16 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B152" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C152" t="s">
         <v>232</v>
       </c>
       <c r="D152">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E152" t="s">
         <v>255</v>
@@ -12170,16 +12173,16 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B153" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C153" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D153">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E153" t="s">
         <v>255</v>
@@ -12187,16 +12190,16 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B154" t="s">
-        <v>140</v>
+        <v>550</v>
       </c>
       <c r="C154" t="s">
         <v>236</v>
       </c>
       <c r="D154">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E154" t="s">
         <v>255</v>
@@ -12204,16 +12207,16 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B155" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C155" t="s">
         <v>236</v>
       </c>
       <c r="D155">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E155" t="s">
         <v>255</v>
@@ -12221,16 +12224,16 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B156" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C156" t="s">
         <v>236</v>
       </c>
       <c r="D156">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E156" t="s">
         <v>255</v>
@@ -12238,16 +12241,16 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B157" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C157" t="s">
         <v>236</v>
       </c>
       <c r="D157">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E157" t="s">
         <v>255</v>
@@ -12255,16 +12258,16 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B158" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C158" t="s">
         <v>236</v>
       </c>
       <c r="D158">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E158" t="s">
         <v>255</v>
@@ -12272,16 +12275,16 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B159" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C159" t="s">
         <v>236</v>
       </c>
       <c r="D159">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E159" t="s">
         <v>255</v>
@@ -12289,16 +12292,16 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B160" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C160" t="s">
-        <v>196</v>
+        <v>236</v>
       </c>
       <c r="D160">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E160" t="s">
         <v>255</v>
@@ -12306,16 +12309,16 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B161" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C161" t="s">
         <v>196</v>
       </c>
       <c r="D161">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E161" t="s">
         <v>255</v>
@@ -12323,16 +12326,16 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B162" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C162" t="s">
         <v>196</v>
       </c>
       <c r="D162">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E162" t="s">
         <v>255</v>
@@ -12340,16 +12343,16 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B163" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C163" t="s">
         <v>196</v>
       </c>
       <c r="D163">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E163" t="s">
         <v>255</v>
@@ -12357,16 +12360,16 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B164" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C164" t="s">
         <v>196</v>
       </c>
       <c r="D164">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E164" t="s">
         <v>255</v>
@@ -12374,16 +12377,16 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B165" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C165" t="s">
         <v>196</v>
       </c>
       <c r="D165">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E165" t="s">
         <v>255</v>
@@ -12391,16 +12394,16 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B166" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C166" t="s">
         <v>196</v>
       </c>
       <c r="D166">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E166" t="s">
         <v>255</v>
@@ -12408,16 +12411,16 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B167" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C167" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="D167">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E167" t="s">
         <v>255</v>
@@ -12425,16 +12428,16 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B168" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C168" t="s">
         <v>216</v>
       </c>
       <c r="D168">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E168" t="s">
         <v>255</v>
@@ -12442,16 +12445,16 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B169" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C169" t="s">
         <v>216</v>
       </c>
       <c r="D169">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E169" t="s">
         <v>255</v>
@@ -12459,16 +12462,16 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B170" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C170" t="s">
         <v>216</v>
       </c>
       <c r="D170">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E170" t="s">
         <v>255</v>
@@ -12476,16 +12479,16 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B171" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C171" t="s">
         <v>216</v>
       </c>
       <c r="D171">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E171" t="s">
         <v>255</v>
@@ -12493,16 +12496,16 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B172" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C172" t="s">
         <v>216</v>
       </c>
       <c r="D172">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E172" t="s">
         <v>255</v>
@@ -12510,16 +12513,16 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B173" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C173" t="s">
         <v>216</v>
       </c>
       <c r="D173">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E173" t="s">
         <v>255</v>
@@ -12527,16 +12530,16 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B174" t="s">
-        <v>551</v>
+        <v>159</v>
       </c>
       <c r="C174" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="D174">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E174" t="s">
         <v>255</v>
@@ -12544,16 +12547,16 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B175" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C175" t="s">
         <v>202</v>
       </c>
       <c r="D175">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E175" t="s">
         <v>255</v>
@@ -12561,16 +12564,16 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B176" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C176" t="s">
         <v>202</v>
       </c>
       <c r="D176">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E176" t="s">
         <v>255</v>
@@ -12578,16 +12581,16 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B177" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C177" t="s">
         <v>202</v>
       </c>
       <c r="D177">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E177" t="s">
         <v>255</v>
@@ -12595,16 +12598,16 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B178" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C178" t="s">
         <v>202</v>
       </c>
       <c r="D178">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E178" t="s">
         <v>255</v>
@@ -12612,16 +12615,16 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B179" t="s">
-        <v>165</v>
+        <v>555</v>
       </c>
       <c r="C179" t="s">
         <v>202</v>
       </c>
       <c r="D179">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E179" t="s">
         <v>255</v>
@@ -12629,16 +12632,16 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B180" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C180" t="s">
         <v>202</v>
       </c>
       <c r="D180">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E180" t="s">
         <v>255</v>
@@ -12646,16 +12649,16 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B181" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C181" t="s">
-        <v>230</v>
+        <v>202</v>
       </c>
       <c r="D181">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E181" t="s">
         <v>255</v>
@@ -12663,16 +12666,16 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B182" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C182" t="s">
         <v>230</v>
       </c>
       <c r="D182">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E182" t="s">
         <v>255</v>
@@ -12680,16 +12683,16 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B183" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C183" t="s">
         <v>230</v>
       </c>
       <c r="D183">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E183" t="s">
         <v>255</v>
@@ -12697,16 +12700,16 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B184" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C184" t="s">
         <v>230</v>
       </c>
       <c r="D184">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E184" t="s">
         <v>255</v>
@@ -12714,16 +12717,16 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B185" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C185" t="s">
         <v>230</v>
       </c>
       <c r="D185">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E185" t="s">
         <v>255</v>
@@ -12731,16 +12734,16 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B186" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C186" t="s">
         <v>230</v>
       </c>
       <c r="D186">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E186" t="s">
         <v>255</v>
@@ -12748,16 +12751,16 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B187" t="s">
-        <v>282</v>
+        <v>172</v>
       </c>
       <c r="C187" t="s">
         <v>230</v>
       </c>
       <c r="D187">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E187" t="s">
         <v>255</v>
@@ -12765,16 +12768,16 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B188" t="s">
-        <v>173</v>
+        <v>282</v>
       </c>
       <c r="C188" t="s">
-        <v>192</v>
+        <v>230</v>
       </c>
       <c r="D188">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="E188" t="s">
         <v>255</v>
@@ -12782,16 +12785,16 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B189" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C189" t="s">
         <v>192</v>
       </c>
       <c r="D189">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E189" t="s">
         <v>255</v>
@@ -12799,16 +12802,16 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B190" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C190" t="s">
         <v>192</v>
       </c>
       <c r="D190">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E190" t="s">
         <v>255</v>
@@ -12816,16 +12819,16 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B191" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C191" t="s">
         <v>192</v>
       </c>
       <c r="D191">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E191" t="s">
         <v>255</v>
@@ -12833,16 +12836,16 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B192" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C192" t="s">
         <v>192</v>
       </c>
       <c r="D192">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E192" t="s">
         <v>255</v>
@@ -12850,16 +12853,16 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B193" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C193" t="s">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="D193">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E193" t="s">
         <v>255</v>
@@ -12867,16 +12870,16 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B194" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C194" t="s">
         <v>218</v>
       </c>
       <c r="D194">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E194" t="s">
         <v>255</v>
@@ -12884,16 +12887,16 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B195" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C195" t="s">
         <v>218</v>
       </c>
       <c r="D195">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E195" t="s">
         <v>255</v>
@@ -12901,16 +12904,16 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B196" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C196" t="s">
         <v>218</v>
       </c>
       <c r="D196">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E196" t="s">
         <v>255</v>
@@ -12918,16 +12921,16 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B197" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C197" t="s">
         <v>218</v>
       </c>
       <c r="D197">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E197" t="s">
         <v>255</v>
@@ -12935,16 +12938,16 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B198" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C198" t="s">
         <v>218</v>
       </c>
       <c r="D198">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E198" t="s">
         <v>255</v>
@@ -12952,16 +12955,16 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B199" t="s">
-        <v>280</v>
+        <v>183</v>
       </c>
       <c r="C199" t="s">
         <v>218</v>
       </c>
       <c r="D199">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E199" t="s">
         <v>255</v>
@@ -12969,16 +12972,16 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B200" t="s">
-        <v>556</v>
+        <v>280</v>
       </c>
       <c r="C200" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="D200">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E200" t="s">
         <v>255</v>
@@ -12986,16 +12989,16 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B201" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C201" t="s">
         <v>210</v>
       </c>
       <c r="D201">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E201" t="s">
         <v>255</v>
@@ -13003,16 +13006,16 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B202" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C202" t="s">
         <v>210</v>
       </c>
       <c r="D202">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E202" t="s">
         <v>255</v>
@@ -13020,16 +13023,16 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B203" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C203" t="s">
         <v>210</v>
       </c>
       <c r="D203">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E203" t="s">
         <v>255</v>
@@ -13037,16 +13040,16 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B204" t="s">
-        <v>188</v>
+        <v>559</v>
       </c>
       <c r="C204" t="s">
         <v>210</v>
       </c>
       <c r="D204">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E204" t="s">
         <v>255</v>
@@ -13054,16 +13057,16 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B205" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C205" t="s">
         <v>210</v>
       </c>
       <c r="D205">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E205" t="s">
         <v>255</v>
@@ -13071,23 +13074,40 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B206" t="s">
-        <v>297</v>
+        <v>189</v>
       </c>
       <c r="C206" t="s">
         <v>210</v>
       </c>
       <c r="D206">
+        <v>2020</v>
+      </c>
+      <c r="E206" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>516</v>
+      </c>
+      <c r="B207" t="s">
+        <v>297</v>
+      </c>
+      <c r="C207" t="s">
+        <v>210</v>
+      </c>
+      <c r="D207">
         <v>2021</v>
       </c>
-      <c r="E206" t="s">
+      <c r="E207" t="s">
         <v>255</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E206" xr:uid="{1CCCF928-8895-4AB9-B900-2E463F961084}"/>
+  <autoFilter ref="A1:E207" xr:uid="{1CCCF928-8895-4AB9-B900-2E463F961084}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
preliminary update of files
</commit_message>
<xml_diff>
--- a/List of Companies and Sustainability Reports.xlsx
+++ b/List of Companies and Sustainability Reports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy Chia\Documents\GitHub\NLP-SustainabilityReports-FinancialPerformance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A38917-3AF8-429F-BB82-CB8D98E4C09A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E919723-7BEB-4CDE-8670-90D3274EB4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Companies" sheetId="2" r:id="rId1"/>
@@ -20,11 +20,11 @@
     <sheet name="Files (New)" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Files (New)'!$A$1:$E$207</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Files (New)'!$A$1:$E$201</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="8" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1565" uniqueCount="564">
   <si>
     <t>ASCENDAS REAL ESTATE INV TRUST_2015_SUS.pdf</t>
   </si>
@@ -1042,24 +1042,6 @@
   </si>
   <si>
     <t>C:\Users\Jeremy Chia\Documents\GitHub\NLP-SustainabilityReports-FinancialPerformance\Sustainability Reports or Annual Reports\CAPITALAND INTEGRATED COMM TR_2021_SUS.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\Jeremy Chia\Documents\GitHub\NLP-SustainabilityReports-FinancialPerformance\Sustainability Reports or Annual Reports\CAPITALAND INVESTMENT LIMITED_2015_SUS.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\Jeremy Chia\Documents\GitHub\NLP-SustainabilityReports-FinancialPerformance\Sustainability Reports or Annual Reports\CAPITALAND INVESTMENT LIMITED_2016_SUS.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\Jeremy Chia\Documents\GitHub\NLP-SustainabilityReports-FinancialPerformance\Sustainability Reports or Annual Reports\CAPITALAND INVESTMENT LIMITED_2017_SUS.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\Jeremy Chia\Documents\GitHub\NLP-SustainabilityReports-FinancialPerformance\Sustainability Reports or Annual Reports\CAPITALAND INVESTMENT LIMITED_2018_SUS.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\Jeremy Chia\Documents\GitHub\NLP-SustainabilityReports-FinancialPerformance\Sustainability Reports or Annual Reports\CAPITALAND INVESTMENT LIMITED_2019_SUS.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\Jeremy Chia\Documents\GitHub\NLP-SustainabilityReports-FinancialPerformance\Sustainability Reports or Annual Reports\CAPITALAND INVESTMENT LIMITED_2020_SUS.pdf</t>
   </si>
   <si>
     <t>C:\Users\Jeremy Chia\Documents\GitHub\NLP-SustainabilityReports-FinancialPerformance\Sustainability Reports or Annual Reports\CAPITALAND INVESTMENT LIMITED_2021_SUS.pdf</t>
@@ -2397,7 +2379,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jeremy Chia" refreshedDate="44815.953209490741" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="206" xr:uid="{FA0BEB66-067C-4621-B92E-AEC381E198A4}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jeremy Chia" refreshedDate="44831.902470949077" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="201" xr:uid="{FA0BEB66-067C-4621-B92E-AEC381E198A4}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B1:E1048576" sheet="Files (New)"/>
   </cacheSource>
@@ -2465,7 +2447,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="206">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="201">
   <r>
     <s v="ASCENDAS REAL ESTATE INV TRUST_2015_SUS.pdf"/>
     <x v="0"/>
@@ -2551,42 +2533,6 @@
     <s v="SUS"/>
   </r>
   <r>
-    <s v="CAPITALAND INVESTMENT LIMITED_2015_SUS.pdf"/>
-    <x v="2"/>
-    <x v="0"/>
-    <s v="SUS"/>
-  </r>
-  <r>
-    <s v="CAPITALAND INVESTMENT LIMITED_2016_SUS.pdf"/>
-    <x v="2"/>
-    <x v="1"/>
-    <s v="SUS"/>
-  </r>
-  <r>
-    <s v="CAPITALAND INVESTMENT LIMITED_2017_SUS.pdf"/>
-    <x v="2"/>
-    <x v="2"/>
-    <s v="SUS"/>
-  </r>
-  <r>
-    <s v="CAPITALAND INVESTMENT LIMITED_2018_SUS.pdf"/>
-    <x v="2"/>
-    <x v="3"/>
-    <s v="SUS"/>
-  </r>
-  <r>
-    <s v="CAPITALAND INVESTMENT LIMITED_2019_SUS.pdf"/>
-    <x v="2"/>
-    <x v="4"/>
-    <s v="SUS"/>
-  </r>
-  <r>
-    <s v="CAPITALAND INVESTMENT LIMITED_2020_SUS.pdf"/>
-    <x v="2"/>
-    <x v="5"/>
-    <s v="SUS"/>
-  </r>
-  <r>
     <s v="CAPITALAND INVESTMENT LIMITED_2021_SUS.pdf"/>
     <x v="2"/>
     <x v="6"/>
@@ -2992,6 +2938,12 @@
     <s v="KEPPEL CORPORATION LIMITED_2020_SUS.pdf"/>
     <x v="12"/>
     <x v="5"/>
+    <s v="SUS"/>
+  </r>
+  <r>
+    <s v="KEPPEL CORPORATION LIMITED_2021_SUS.pdf"/>
+    <x v="12"/>
+    <x v="6"/>
     <s v="SUS"/>
   </r>
   <r>
@@ -3706,7 +3658,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BE24C027-C167-4BA0-A791-AD3E10842C2F}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BE24C027-C167-4BA0-A791-AD3E10842C2F}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:J36" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0"/>
@@ -6920,7 +6872,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="B90" t="s">
         <v>198</v>
@@ -8582,8 +8534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F4E8A3B-D84D-448A-8B88-7C60596CA3BA}">
   <dimension ref="A3:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8597,15 +8549,15 @@
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="B4">
         <v>2015</v>
@@ -8629,10 +8581,10 @@
         <v>2021</v>
       </c>
       <c r="I4" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="J4" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -8699,30 +8651,18 @@
       <c r="A7" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B7" s="8">
-        <v>1</v>
-      </c>
-      <c r="C7" s="8">
-        <v>1</v>
-      </c>
-      <c r="D7" s="8">
-        <v>1</v>
-      </c>
-      <c r="E7" s="8">
-        <v>1</v>
-      </c>
-      <c r="F7" s="8">
-        <v>1</v>
-      </c>
-      <c r="G7" s="8">
-        <v>1</v>
-      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
       <c r="H7" s="8">
         <v>1</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -9013,10 +8953,12 @@
       <c r="G17" s="8">
         <v>1</v>
       </c>
-      <c r="H17" s="8"/>
+      <c r="H17" s="8">
+        <v>1</v>
+      </c>
       <c r="I17" s="8"/>
       <c r="J17" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -9527,7 +9469,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -9541,32 +9483,32 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="B36" s="8">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C36" s="8">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D36" s="8">
+        <v>29</v>
+      </c>
+      <c r="E36" s="8">
+        <v>29</v>
+      </c>
+      <c r="F36" s="8">
+        <v>29</v>
+      </c>
+      <c r="G36" s="8">
+        <v>29</v>
+      </c>
+      <c r="H36" s="8">
         <v>30</v>
-      </c>
-      <c r="E36" s="8">
-        <v>30</v>
-      </c>
-      <c r="F36" s="8">
-        <v>30</v>
-      </c>
-      <c r="G36" s="8">
-        <v>30</v>
-      </c>
-      <c r="H36" s="8">
-        <v>29</v>
       </c>
       <c r="I36" s="8"/>
       <c r="J36" s="8">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -9576,23 +9518,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCCF928-8895-4AB9-B900-2E463F961084}">
-  <dimension ref="A1:E207"/>
+  <dimension ref="A1:E201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
-      <selection sqref="A1:E207"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="B1" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="C1" t="s">
         <v>253</v>
@@ -9601,7 +9544,7 @@
         <v>254</v>
       </c>
       <c r="E1" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -9728,7 +9671,7 @@
         <v>319</v>
       </c>
       <c r="B9" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="C9" t="s">
         <v>200</v>
@@ -9745,7 +9688,7 @@
         <v>320</v>
       </c>
       <c r="B10" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="C10" t="s">
         <v>200</v>
@@ -9762,7 +9705,7 @@
         <v>321</v>
       </c>
       <c r="B11" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="C11" t="s">
         <v>200</v>
@@ -9779,7 +9722,7 @@
         <v>322</v>
       </c>
       <c r="B12" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="C12" t="s">
         <v>200</v>
@@ -9796,7 +9739,7 @@
         <v>323</v>
       </c>
       <c r="B13" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="C13" t="s">
         <v>200</v>
@@ -9813,7 +9756,7 @@
         <v>324</v>
       </c>
       <c r="B14" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="C14" t="s">
         <v>200</v>
@@ -9830,7 +9773,7 @@
         <v>325</v>
       </c>
       <c r="B15" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="C15" t="s">
         <v>200</v>
@@ -9847,13 +9790,13 @@
         <v>326</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>272</v>
       </c>
       <c r="C16" t="s">
         <v>212</v>
       </c>
       <c r="D16">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E16" t="s">
         <v>255</v>
@@ -9864,13 +9807,13 @@
         <v>327</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="D17">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E17" t="s">
         <v>255</v>
@@ -9881,13 +9824,13 @@
         <v>328</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="D18">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E18" t="s">
         <v>255</v>
@@ -9898,13 +9841,13 @@
         <v>329</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="D19">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E19" t="s">
         <v>255</v>
@@ -9915,13 +9858,13 @@
         <v>330</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="D20">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E20" t="s">
         <v>255</v>
@@ -9932,13 +9875,13 @@
         <v>331</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="D21">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E21" t="s">
         <v>255</v>
@@ -9949,13 +9892,13 @@
         <v>332</v>
       </c>
       <c r="B22" t="s">
-        <v>272</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="D22">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E22" t="s">
         <v>255</v>
@@ -9966,13 +9909,13 @@
         <v>333</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
         <v>224</v>
       </c>
       <c r="D23">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E23" t="s">
         <v>255</v>
@@ -9983,13 +9926,13 @@
         <v>334</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>224</v>
+        <v>190</v>
       </c>
       <c r="D24">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E24" t="s">
         <v>255</v>
@@ -10000,13 +9943,13 @@
         <v>335</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>224</v>
+        <v>190</v>
       </c>
       <c r="D25">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E25" t="s">
         <v>255</v>
@@ -10017,13 +9960,13 @@
         <v>336</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>224</v>
+        <v>190</v>
       </c>
       <c r="D26">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E26" t="s">
         <v>255</v>
@@ -10034,13 +9977,13 @@
         <v>337</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>224</v>
+        <v>190</v>
       </c>
       <c r="D27">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E27" t="s">
         <v>255</v>
@@ -10051,13 +9994,13 @@
         <v>338</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>224</v>
+        <v>190</v>
       </c>
       <c r="D28">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E28" t="s">
         <v>255</v>
@@ -10068,13 +10011,13 @@
         <v>339</v>
       </c>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>224</v>
+        <v>190</v>
       </c>
       <c r="D29">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E29" t="s">
         <v>255</v>
@@ -10085,13 +10028,13 @@
         <v>340</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s">
         <v>190</v>
       </c>
       <c r="D30">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E30" t="s">
         <v>255</v>
@@ -10102,13 +10045,13 @@
         <v>341</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>518</v>
       </c>
       <c r="C31" t="s">
-        <v>190</v>
+        <v>240</v>
       </c>
       <c r="D31">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E31" t="s">
         <v>255</v>
@@ -10119,13 +10062,13 @@
         <v>342</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>519</v>
       </c>
       <c r="C32" t="s">
-        <v>190</v>
+        <v>240</v>
       </c>
       <c r="D32">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E32" t="s">
         <v>255</v>
@@ -10136,13 +10079,13 @@
         <v>343</v>
       </c>
       <c r="B33" t="s">
-        <v>26</v>
+        <v>520</v>
       </c>
       <c r="C33" t="s">
-        <v>190</v>
+        <v>240</v>
       </c>
       <c r="D33">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E33" t="s">
         <v>255</v>
@@ -10153,13 +10096,13 @@
         <v>344</v>
       </c>
       <c r="B34" t="s">
-        <v>27</v>
+        <v>521</v>
       </c>
       <c r="C34" t="s">
-        <v>190</v>
+        <v>240</v>
       </c>
       <c r="D34">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E34" t="s">
         <v>255</v>
@@ -10170,13 +10113,13 @@
         <v>345</v>
       </c>
       <c r="B35" t="s">
-        <v>28</v>
+        <v>522</v>
       </c>
       <c r="C35" t="s">
-        <v>190</v>
+        <v>240</v>
       </c>
       <c r="D35">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E35" t="s">
         <v>255</v>
@@ -10187,13 +10130,13 @@
         <v>346</v>
       </c>
       <c r="B36" t="s">
-        <v>29</v>
+        <v>523</v>
       </c>
       <c r="C36" t="s">
-        <v>190</v>
+        <v>240</v>
       </c>
       <c r="D36">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E36" t="s">
         <v>255</v>
@@ -10210,7 +10153,7 @@
         <v>240</v>
       </c>
       <c r="D37">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E37" t="s">
         <v>255</v>
@@ -10221,13 +10164,13 @@
         <v>348</v>
       </c>
       <c r="B38" t="s">
-        <v>525</v>
+        <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>240</v>
+        <v>194</v>
       </c>
       <c r="D38">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E38" t="s">
         <v>255</v>
@@ -10238,13 +10181,13 @@
         <v>349</v>
       </c>
       <c r="B39" t="s">
-        <v>526</v>
+        <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>240</v>
+        <v>194</v>
       </c>
       <c r="D39">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E39" t="s">
         <v>255</v>
@@ -10255,13 +10198,13 @@
         <v>350</v>
       </c>
       <c r="B40" t="s">
-        <v>527</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>240</v>
+        <v>194</v>
       </c>
       <c r="D40">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E40" t="s">
         <v>255</v>
@@ -10272,13 +10215,13 @@
         <v>351</v>
       </c>
       <c r="B41" t="s">
-        <v>528</v>
+        <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>240</v>
+        <v>194</v>
       </c>
       <c r="D41">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E41" t="s">
         <v>255</v>
@@ -10289,13 +10232,13 @@
         <v>352</v>
       </c>
       <c r="B42" t="s">
-        <v>529</v>
+        <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>240</v>
+        <v>194</v>
       </c>
       <c r="D42">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E42" t="s">
         <v>255</v>
@@ -10306,13 +10249,13 @@
         <v>353</v>
       </c>
       <c r="B43" t="s">
-        <v>530</v>
+        <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>240</v>
+        <v>194</v>
       </c>
       <c r="D43">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E43" t="s">
         <v>255</v>
@@ -10323,13 +10266,13 @@
         <v>354</v>
       </c>
       <c r="B44" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C44" t="s">
         <v>194</v>
       </c>
       <c r="D44">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E44" t="s">
         <v>255</v>
@@ -10340,13 +10283,13 @@
         <v>355</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>273</v>
       </c>
       <c r="C45" t="s">
-        <v>194</v>
+        <v>238</v>
       </c>
       <c r="D45">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="E45" t="s">
         <v>255</v>
@@ -10357,13 +10300,13 @@
         <v>356</v>
       </c>
       <c r="B46" t="s">
-        <v>39</v>
+        <v>274</v>
       </c>
       <c r="C46" t="s">
-        <v>194</v>
+        <v>238</v>
       </c>
       <c r="D46">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="E46" t="s">
         <v>255</v>
@@ -10374,13 +10317,13 @@
         <v>357</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
+        <v>275</v>
       </c>
       <c r="C47" t="s">
-        <v>194</v>
+        <v>238</v>
       </c>
       <c r="D47">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="E47" t="s">
         <v>255</v>
@@ -10391,13 +10334,13 @@
         <v>358</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>276</v>
       </c>
       <c r="C48" t="s">
-        <v>194</v>
+        <v>238</v>
       </c>
       <c r="D48">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="E48" t="s">
         <v>255</v>
@@ -10408,13 +10351,13 @@
         <v>359</v>
       </c>
       <c r="B49" t="s">
-        <v>42</v>
+        <v>277</v>
       </c>
       <c r="C49" t="s">
-        <v>194</v>
+        <v>238</v>
       </c>
       <c r="D49">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E49" t="s">
         <v>255</v>
@@ -10425,13 +10368,13 @@
         <v>360</v>
       </c>
       <c r="B50" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C50" t="s">
-        <v>194</v>
+        <v>234</v>
       </c>
       <c r="D50">
-        <v>2021</v>
+        <v>2015</v>
       </c>
       <c r="E50" t="s">
         <v>255</v>
@@ -10442,13 +10385,13 @@
         <v>361</v>
       </c>
       <c r="B51" t="s">
-        <v>273</v>
+        <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D51">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E51" t="s">
         <v>255</v>
@@ -10459,13 +10402,13 @@
         <v>362</v>
       </c>
       <c r="B52" t="s">
-        <v>274</v>
+        <v>46</v>
       </c>
       <c r="C52" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D52">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E52" t="s">
         <v>255</v>
@@ -10476,13 +10419,13 @@
         <v>363</v>
       </c>
       <c r="B53" t="s">
-        <v>275</v>
+        <v>47</v>
       </c>
       <c r="C53" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D53">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E53" t="s">
         <v>255</v>
@@ -10493,13 +10436,13 @@
         <v>364</v>
       </c>
       <c r="B54" t="s">
-        <v>276</v>
+        <v>48</v>
       </c>
       <c r="C54" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D54">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E54" t="s">
         <v>255</v>
@@ -10510,13 +10453,13 @@
         <v>365</v>
       </c>
       <c r="B55" t="s">
-        <v>277</v>
+        <v>49</v>
       </c>
       <c r="C55" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D55">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E55" t="s">
         <v>255</v>
@@ -10527,13 +10470,13 @@
         <v>366</v>
       </c>
       <c r="B56" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C56" t="s">
         <v>234</v>
       </c>
       <c r="D56">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E56" t="s">
         <v>255</v>
@@ -10544,13 +10487,13 @@
         <v>367</v>
       </c>
       <c r="B57" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C57" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="D57">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E57" t="s">
         <v>255</v>
@@ -10561,13 +10504,13 @@
         <v>368</v>
       </c>
       <c r="B58" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C58" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="D58">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E58" t="s">
         <v>255</v>
@@ -10578,13 +10521,13 @@
         <v>369</v>
       </c>
       <c r="B59" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C59" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="D59">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E59" t="s">
         <v>255</v>
@@ -10595,13 +10538,13 @@
         <v>370</v>
       </c>
       <c r="B60" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C60" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="D60">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E60" t="s">
         <v>255</v>
@@ -10612,13 +10555,13 @@
         <v>371</v>
       </c>
       <c r="B61" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C61" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="D61">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E61" t="s">
         <v>255</v>
@@ -10629,13 +10572,13 @@
         <v>372</v>
       </c>
       <c r="B62" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C62" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="D62">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E62" t="s">
         <v>255</v>
@@ -10646,13 +10589,13 @@
         <v>373</v>
       </c>
       <c r="B63" t="s">
-        <v>51</v>
+        <v>278</v>
       </c>
       <c r="C63" t="s">
         <v>244</v>
       </c>
       <c r="D63">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E63" t="s">
         <v>255</v>
@@ -10663,13 +10606,13 @@
         <v>374</v>
       </c>
       <c r="B64" t="s">
-        <v>52</v>
+        <v>525</v>
       </c>
       <c r="C64" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D64">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E64" t="s">
         <v>255</v>
@@ -10680,13 +10623,13 @@
         <v>375</v>
       </c>
       <c r="B65" t="s">
-        <v>53</v>
+        <v>526</v>
       </c>
       <c r="C65" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D65">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E65" t="s">
         <v>255</v>
@@ -10697,13 +10640,13 @@
         <v>376</v>
       </c>
       <c r="B66" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C66" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D66">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E66" t="s">
         <v>255</v>
@@ -10714,13 +10657,13 @@
         <v>377</v>
       </c>
       <c r="B67" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C67" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D67">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E67" t="s">
         <v>255</v>
@@ -10731,13 +10674,13 @@
         <v>378</v>
       </c>
       <c r="B68" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C68" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D68">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E68" t="s">
         <v>255</v>
@@ -10748,13 +10691,13 @@
         <v>379</v>
       </c>
       <c r="B69" t="s">
-        <v>278</v>
+        <v>62</v>
       </c>
       <c r="C69" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D69">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E69" t="s">
         <v>255</v>
@@ -10765,13 +10708,13 @@
         <v>380</v>
       </c>
       <c r="B70" t="s">
-        <v>531</v>
+        <v>279</v>
       </c>
       <c r="C70" t="s">
         <v>246</v>
       </c>
       <c r="D70">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E70" t="s">
         <v>255</v>
@@ -10782,13 +10725,13 @@
         <v>381</v>
       </c>
       <c r="B71" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="C71" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D71">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E71" t="s">
         <v>255</v>
@@ -10799,13 +10742,13 @@
         <v>382</v>
       </c>
       <c r="B72" t="s">
-        <v>59</v>
+        <v>528</v>
       </c>
       <c r="C72" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D72">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E72" t="s">
         <v>255</v>
@@ -10816,13 +10759,13 @@
         <v>383</v>
       </c>
       <c r="B73" t="s">
-        <v>60</v>
+        <v>529</v>
       </c>
       <c r="C73" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D73">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E73" t="s">
         <v>255</v>
@@ -10833,13 +10776,13 @@
         <v>384</v>
       </c>
       <c r="B74" t="s">
-        <v>61</v>
+        <v>530</v>
       </c>
       <c r="C74" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D74">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E74" t="s">
         <v>255</v>
@@ -10850,13 +10793,13 @@
         <v>385</v>
       </c>
       <c r="B75" t="s">
-        <v>62</v>
+        <v>531</v>
       </c>
       <c r="C75" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D75">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E75" t="s">
         <v>255</v>
@@ -10867,13 +10810,13 @@
         <v>386</v>
       </c>
       <c r="B76" t="s">
-        <v>279</v>
+        <v>68</v>
       </c>
       <c r="C76" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D76">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E76" t="s">
         <v>255</v>
@@ -10884,13 +10827,13 @@
         <v>387</v>
       </c>
       <c r="B77" t="s">
-        <v>533</v>
+        <v>69</v>
       </c>
       <c r="C77" t="s">
         <v>248</v>
       </c>
       <c r="D77">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E77" t="s">
         <v>255</v>
@@ -10901,13 +10844,13 @@
         <v>388</v>
       </c>
       <c r="B78" t="s">
-        <v>534</v>
+        <v>70</v>
       </c>
       <c r="C78" t="s">
-        <v>248</v>
+        <v>198</v>
       </c>
       <c r="D78">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E78" t="s">
         <v>255</v>
@@ -10918,13 +10861,13 @@
         <v>389</v>
       </c>
       <c r="B79" t="s">
-        <v>535</v>
+        <v>71</v>
       </c>
       <c r="C79" t="s">
-        <v>248</v>
+        <v>198</v>
       </c>
       <c r="D79">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E79" t="s">
         <v>255</v>
@@ -10935,13 +10878,13 @@
         <v>390</v>
       </c>
       <c r="B80" t="s">
-        <v>536</v>
+        <v>72</v>
       </c>
       <c r="C80" t="s">
-        <v>248</v>
+        <v>198</v>
       </c>
       <c r="D80">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E80" t="s">
         <v>255</v>
@@ -10952,13 +10895,13 @@
         <v>391</v>
       </c>
       <c r="B81" t="s">
-        <v>537</v>
+        <v>73</v>
       </c>
       <c r="C81" t="s">
-        <v>248</v>
+        <v>198</v>
       </c>
       <c r="D81">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E81" t="s">
         <v>255</v>
@@ -10969,13 +10912,13 @@
         <v>392</v>
       </c>
       <c r="B82" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C82" t="s">
-        <v>248</v>
+        <v>198</v>
       </c>
       <c r="D82">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E82" t="s">
         <v>255</v>
@@ -10986,13 +10929,13 @@
         <v>393</v>
       </c>
       <c r="B83" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C83" t="s">
-        <v>248</v>
+        <v>198</v>
       </c>
       <c r="D83">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E83" t="s">
         <v>255</v>
@@ -11000,16 +10943,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>394</v>
+        <v>563</v>
       </c>
       <c r="B84" t="s">
-        <v>70</v>
+        <v>562</v>
       </c>
       <c r="C84" t="s">
         <v>198</v>
       </c>
       <c r="D84">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E84" t="s">
         <v>255</v>
@@ -11017,16 +10960,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B85" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C85" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="D85">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E85" t="s">
         <v>255</v>
@@ -11034,16 +10977,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B86" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C86" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="D86">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E86" t="s">
         <v>255</v>
@@ -11051,16 +10994,16 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B87" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C87" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="D87">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E87" t="s">
         <v>255</v>
@@ -11068,16 +11011,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B88" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C88" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="D88">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E88" t="s">
         <v>255</v>
@@ -11085,16 +11028,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B89" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C89" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="D89">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E89" t="s">
         <v>255</v>
@@ -11102,16 +11045,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>569</v>
+        <v>399</v>
       </c>
       <c r="B90" t="s">
-        <v>568</v>
+        <v>81</v>
       </c>
       <c r="C90" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="D90">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E90" t="s">
         <v>255</v>
@@ -11122,13 +11065,13 @@
         <v>400</v>
       </c>
       <c r="B91" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C91" t="s">
         <v>222</v>
       </c>
       <c r="D91">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E91" t="s">
         <v>255</v>
@@ -11139,13 +11082,13 @@
         <v>401</v>
       </c>
       <c r="B92" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C92" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="D92">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E92" t="s">
         <v>255</v>
@@ -11156,13 +11099,13 @@
         <v>402</v>
       </c>
       <c r="B93" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C93" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="D93">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E93" t="s">
         <v>255</v>
@@ -11173,13 +11116,13 @@
         <v>403</v>
       </c>
       <c r="B94" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C94" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="D94">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E94" t="s">
         <v>255</v>
@@ -11190,13 +11133,13 @@
         <v>404</v>
       </c>
       <c r="B95" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C95" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="D95">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E95" t="s">
         <v>255</v>
@@ -11207,13 +11150,13 @@
         <v>405</v>
       </c>
       <c r="B96" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C96" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="D96">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E96" t="s">
         <v>255</v>
@@ -11224,13 +11167,13 @@
         <v>406</v>
       </c>
       <c r="B97" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C97" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="D97">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E97" t="s">
         <v>255</v>
@@ -11241,13 +11184,13 @@
         <v>407</v>
       </c>
       <c r="B98" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C98" t="s">
         <v>214</v>
       </c>
       <c r="D98">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E98" t="s">
         <v>255</v>
@@ -11258,13 +11201,13 @@
         <v>408</v>
       </c>
       <c r="B99" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C99" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D99">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E99" t="s">
         <v>255</v>
@@ -11275,13 +11218,13 @@
         <v>409</v>
       </c>
       <c r="B100" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C100" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D100">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E100" t="s">
         <v>255</v>
@@ -11292,13 +11235,13 @@
         <v>410</v>
       </c>
       <c r="B101" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C101" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D101">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E101" t="s">
         <v>255</v>
@@ -11309,13 +11252,13 @@
         <v>411</v>
       </c>
       <c r="B102" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C102" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D102">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E102" t="s">
         <v>255</v>
@@ -11326,13 +11269,13 @@
         <v>412</v>
       </c>
       <c r="B103" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C103" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D103">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E103" t="s">
         <v>255</v>
@@ -11343,13 +11286,13 @@
         <v>413</v>
       </c>
       <c r="B104" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C104" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D104">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E104" t="s">
         <v>255</v>
@@ -11360,13 +11303,13 @@
         <v>414</v>
       </c>
       <c r="B105" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C105" t="s">
         <v>220</v>
       </c>
       <c r="D105">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E105" t="s">
         <v>255</v>
@@ -11377,13 +11320,13 @@
         <v>415</v>
       </c>
       <c r="B106" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C106" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="D106">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E106" t="s">
         <v>255</v>
@@ -11394,13 +11337,13 @@
         <v>416</v>
       </c>
       <c r="B107" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C107" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="D107">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E107" t="s">
         <v>255</v>
@@ -11411,13 +11354,13 @@
         <v>417</v>
       </c>
       <c r="B108" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C108" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="D108">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E108" t="s">
         <v>255</v>
@@ -11428,13 +11371,13 @@
         <v>418</v>
       </c>
       <c r="B109" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C109" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="D109">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E109" t="s">
         <v>255</v>
@@ -11445,13 +11388,13 @@
         <v>419</v>
       </c>
       <c r="B110" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C110" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="D110">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E110" t="s">
         <v>255</v>
@@ -11462,13 +11405,13 @@
         <v>420</v>
       </c>
       <c r="B111" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C111" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="D111">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E111" t="s">
         <v>255</v>
@@ -11479,13 +11422,13 @@
         <v>421</v>
       </c>
       <c r="B112" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C112" t="s">
         <v>204</v>
       </c>
       <c r="D112">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E112" t="s">
         <v>255</v>
@@ -11496,13 +11439,13 @@
         <v>422</v>
       </c>
       <c r="B113" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C113" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D113">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E113" t="s">
         <v>255</v>
@@ -11513,13 +11456,13 @@
         <v>423</v>
       </c>
       <c r="B114" t="s">
-        <v>99</v>
+        <v>532</v>
       </c>
       <c r="C114" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D114">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E114" t="s">
         <v>255</v>
@@ -11530,13 +11473,13 @@
         <v>424</v>
       </c>
       <c r="B115" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C115" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D115">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E115" t="s">
         <v>255</v>
@@ -11547,13 +11490,13 @@
         <v>425</v>
       </c>
       <c r="B116" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C116" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D116">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E116" t="s">
         <v>255</v>
@@ -11564,13 +11507,13 @@
         <v>426</v>
       </c>
       <c r="B117" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C117" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D117">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E117" t="s">
         <v>255</v>
@@ -11581,13 +11524,13 @@
         <v>427</v>
       </c>
       <c r="B118" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C118" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D118">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E118" t="s">
         <v>255</v>
@@ -11598,13 +11541,13 @@
         <v>428</v>
       </c>
       <c r="B119" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C119" t="s">
         <v>208</v>
       </c>
       <c r="D119">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E119" t="s">
         <v>255</v>
@@ -11615,13 +11558,13 @@
         <v>429</v>
       </c>
       <c r="B120" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="C120" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="D120">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E120" t="s">
         <v>255</v>
@@ -11632,13 +11575,13 @@
         <v>430</v>
       </c>
       <c r="B121" t="s">
-        <v>106</v>
+        <v>534</v>
       </c>
       <c r="C121" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="D121">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E121" t="s">
         <v>255</v>
@@ -11649,13 +11592,13 @@
         <v>431</v>
       </c>
       <c r="B122" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C122" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="D122">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E122" t="s">
         <v>255</v>
@@ -11666,13 +11609,13 @@
         <v>432</v>
       </c>
       <c r="B123" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C123" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="D123">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E123" t="s">
         <v>255</v>
@@ -11683,13 +11626,13 @@
         <v>433</v>
       </c>
       <c r="B124" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C124" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="D124">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E124" t="s">
         <v>255</v>
@@ -11700,13 +11643,13 @@
         <v>434</v>
       </c>
       <c r="B125" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C125" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="D125">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E125" t="s">
         <v>255</v>
@@ -11717,13 +11660,13 @@
         <v>435</v>
       </c>
       <c r="B126" t="s">
-        <v>539</v>
+        <v>117</v>
       </c>
       <c r="C126" t="s">
         <v>228</v>
       </c>
       <c r="D126">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E126" t="s">
         <v>255</v>
@@ -11734,13 +11677,13 @@
         <v>436</v>
       </c>
       <c r="B127" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="C127" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D127">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E127" t="s">
         <v>255</v>
@@ -11751,13 +11694,13 @@
         <v>437</v>
       </c>
       <c r="B128" t="s">
-        <v>113</v>
+        <v>536</v>
       </c>
       <c r="C128" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D128">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E128" t="s">
         <v>255</v>
@@ -11768,13 +11711,13 @@
         <v>438</v>
       </c>
       <c r="B129" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C129" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D129">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E129" t="s">
         <v>255</v>
@@ -11785,13 +11728,13 @@
         <v>439</v>
       </c>
       <c r="B130" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C130" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D130">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E130" t="s">
         <v>255</v>
@@ -11802,13 +11745,13 @@
         <v>440</v>
       </c>
       <c r="B131" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C131" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D131">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E131" t="s">
         <v>255</v>
@@ -11819,13 +11762,13 @@
         <v>441</v>
       </c>
       <c r="B132" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C132" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D132">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E132" t="s">
         <v>255</v>
@@ -11836,13 +11779,13 @@
         <v>442</v>
       </c>
       <c r="B133" t="s">
-        <v>541</v>
+        <v>124</v>
       </c>
       <c r="C133" t="s">
         <v>226</v>
       </c>
       <c r="D133">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E133" t="s">
         <v>255</v>
@@ -11853,13 +11796,13 @@
         <v>443</v>
       </c>
       <c r="B134" t="s">
-        <v>542</v>
+        <v>125</v>
       </c>
       <c r="C134" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="D134">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E134" t="s">
         <v>255</v>
@@ -11870,13 +11813,13 @@
         <v>444</v>
       </c>
       <c r="B135" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C135" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="D135">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E135" t="s">
         <v>255</v>
@@ -11887,13 +11830,13 @@
         <v>445</v>
       </c>
       <c r="B136" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C136" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="D136">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E136" t="s">
         <v>255</v>
@@ -11904,13 +11847,13 @@
         <v>446</v>
       </c>
       <c r="B137" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C137" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="D137">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E137" t="s">
         <v>255</v>
@@ -11921,13 +11864,13 @@
         <v>447</v>
       </c>
       <c r="B138" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C138" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="D138">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E138" t="s">
         <v>255</v>
@@ -11938,13 +11881,13 @@
         <v>448</v>
       </c>
       <c r="B139" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C139" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="D139">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E139" t="s">
         <v>255</v>
@@ -11955,13 +11898,13 @@
         <v>449</v>
       </c>
       <c r="B140" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C140" t="s">
         <v>242</v>
       </c>
       <c r="D140">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E140" t="s">
         <v>255</v>
@@ -11972,13 +11915,13 @@
         <v>450</v>
       </c>
       <c r="B141" t="s">
-        <v>126</v>
+        <v>537</v>
       </c>
       <c r="C141" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="D141">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E141" t="s">
         <v>255</v>
@@ -11989,13 +11932,13 @@
         <v>451</v>
       </c>
       <c r="B142" t="s">
-        <v>127</v>
+        <v>538</v>
       </c>
       <c r="C142" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="D142">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E142" t="s">
         <v>255</v>
@@ -12006,13 +11949,13 @@
         <v>452</v>
       </c>
       <c r="B143" t="s">
-        <v>128</v>
+        <v>539</v>
       </c>
       <c r="C143" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="D143">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E143" t="s">
         <v>255</v>
@@ -12023,13 +11966,13 @@
         <v>453</v>
       </c>
       <c r="B144" t="s">
-        <v>129</v>
+        <v>540</v>
       </c>
       <c r="C144" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="D144">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E144" t="s">
         <v>255</v>
@@ -12040,13 +11983,13 @@
         <v>454</v>
       </c>
       <c r="B145" t="s">
-        <v>130</v>
+        <v>541</v>
       </c>
       <c r="C145" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="D145">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E145" t="s">
         <v>255</v>
@@ -12057,13 +12000,13 @@
         <v>455</v>
       </c>
       <c r="B146" t="s">
-        <v>131</v>
+        <v>542</v>
       </c>
       <c r="C146" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="D146">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E146" t="s">
         <v>255</v>
@@ -12080,7 +12023,7 @@
         <v>232</v>
       </c>
       <c r="D147">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E147" t="s">
         <v>255</v>
@@ -12094,10 +12037,10 @@
         <v>544</v>
       </c>
       <c r="C148" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D148">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E148" t="s">
         <v>255</v>
@@ -12108,13 +12051,13 @@
         <v>458</v>
       </c>
       <c r="B149" t="s">
-        <v>545</v>
+        <v>140</v>
       </c>
       <c r="C149" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D149">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E149" t="s">
         <v>255</v>
@@ -12125,13 +12068,13 @@
         <v>459</v>
       </c>
       <c r="B150" t="s">
-        <v>546</v>
+        <v>141</v>
       </c>
       <c r="C150" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D150">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E150" t="s">
         <v>255</v>
@@ -12142,13 +12085,13 @@
         <v>460</v>
       </c>
       <c r="B151" t="s">
-        <v>547</v>
+        <v>142</v>
       </c>
       <c r="C151" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D151">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E151" t="s">
         <v>255</v>
@@ -12159,13 +12102,13 @@
         <v>461</v>
       </c>
       <c r="B152" t="s">
-        <v>548</v>
+        <v>143</v>
       </c>
       <c r="C152" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D152">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E152" t="s">
         <v>255</v>
@@ -12176,13 +12119,13 @@
         <v>462</v>
       </c>
       <c r="B153" t="s">
-        <v>549</v>
+        <v>144</v>
       </c>
       <c r="C153" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D153">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E153" t="s">
         <v>255</v>
@@ -12193,13 +12136,13 @@
         <v>463</v>
       </c>
       <c r="B154" t="s">
-        <v>550</v>
+        <v>145</v>
       </c>
       <c r="C154" t="s">
         <v>236</v>
       </c>
       <c r="D154">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E154" t="s">
         <v>255</v>
@@ -12210,13 +12153,13 @@
         <v>464</v>
       </c>
       <c r="B155" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C155" t="s">
-        <v>236</v>
+        <v>196</v>
       </c>
       <c r="D155">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E155" t="s">
         <v>255</v>
@@ -12227,13 +12170,13 @@
         <v>465</v>
       </c>
       <c r="B156" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C156" t="s">
-        <v>236</v>
+        <v>196</v>
       </c>
       <c r="D156">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E156" t="s">
         <v>255</v>
@@ -12244,13 +12187,13 @@
         <v>466</v>
       </c>
       <c r="B157" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C157" t="s">
-        <v>236</v>
+        <v>196</v>
       </c>
       <c r="D157">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E157" t="s">
         <v>255</v>
@@ -12261,13 +12204,13 @@
         <v>467</v>
       </c>
       <c r="B158" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C158" t="s">
-        <v>236</v>
+        <v>196</v>
       </c>
       <c r="D158">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E158" t="s">
         <v>255</v>
@@ -12278,13 +12221,13 @@
         <v>468</v>
       </c>
       <c r="B159" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C159" t="s">
-        <v>236</v>
+        <v>196</v>
       </c>
       <c r="D159">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E159" t="s">
         <v>255</v>
@@ -12295,13 +12238,13 @@
         <v>469</v>
       </c>
       <c r="B160" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C160" t="s">
-        <v>236</v>
+        <v>196</v>
       </c>
       <c r="D160">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E160" t="s">
         <v>255</v>
@@ -12312,13 +12255,13 @@
         <v>470</v>
       </c>
       <c r="B161" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C161" t="s">
         <v>196</v>
       </c>
       <c r="D161">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E161" t="s">
         <v>255</v>
@@ -12329,13 +12272,13 @@
         <v>471</v>
       </c>
       <c r="B162" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C162" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="D162">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E162" t="s">
         <v>255</v>
@@ -12346,13 +12289,13 @@
         <v>472</v>
       </c>
       <c r="B163" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C163" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="D163">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E163" t="s">
         <v>255</v>
@@ -12363,13 +12306,13 @@
         <v>473</v>
       </c>
       <c r="B164" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C164" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="D164">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E164" t="s">
         <v>255</v>
@@ -12380,13 +12323,13 @@
         <v>474</v>
       </c>
       <c r="B165" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="C165" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="D165">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E165" t="s">
         <v>255</v>
@@ -12397,13 +12340,13 @@
         <v>475</v>
       </c>
       <c r="B166" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C166" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="D166">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E166" t="s">
         <v>255</v>
@@ -12414,13 +12357,13 @@
         <v>476</v>
       </c>
       <c r="B167" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="C167" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="D167">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E167" t="s">
         <v>255</v>
@@ -12431,13 +12374,13 @@
         <v>477</v>
       </c>
       <c r="B168" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C168" t="s">
         <v>216</v>
       </c>
       <c r="D168">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E168" t="s">
         <v>255</v>
@@ -12448,13 +12391,13 @@
         <v>478</v>
       </c>
       <c r="B169" t="s">
-        <v>154</v>
+        <v>545</v>
       </c>
       <c r="C169" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="D169">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E169" t="s">
         <v>255</v>
@@ -12465,13 +12408,13 @@
         <v>479</v>
       </c>
       <c r="B170" t="s">
-        <v>155</v>
+        <v>546</v>
       </c>
       <c r="C170" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="D170">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E170" t="s">
         <v>255</v>
@@ -12482,13 +12425,13 @@
         <v>480</v>
       </c>
       <c r="B171" t="s">
-        <v>156</v>
+        <v>547</v>
       </c>
       <c r="C171" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="D171">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E171" t="s">
         <v>255</v>
@@ -12499,13 +12442,13 @@
         <v>481</v>
       </c>
       <c r="B172" t="s">
-        <v>157</v>
+        <v>548</v>
       </c>
       <c r="C172" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="D172">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E172" t="s">
         <v>255</v>
@@ -12516,13 +12459,13 @@
         <v>482</v>
       </c>
       <c r="B173" t="s">
-        <v>158</v>
+        <v>549</v>
       </c>
       <c r="C173" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="D173">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E173" t="s">
         <v>255</v>
@@ -12533,13 +12476,13 @@
         <v>483</v>
       </c>
       <c r="B174" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C174" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="D174">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E174" t="s">
         <v>255</v>
@@ -12550,13 +12493,13 @@
         <v>484</v>
       </c>
       <c r="B175" t="s">
-        <v>551</v>
+        <v>166</v>
       </c>
       <c r="C175" t="s">
         <v>202</v>
       </c>
       <c r="D175">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E175" t="s">
         <v>255</v>
@@ -12567,13 +12510,13 @@
         <v>485</v>
       </c>
       <c r="B176" t="s">
-        <v>552</v>
+        <v>167</v>
       </c>
       <c r="C176" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="D176">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E176" t="s">
         <v>255</v>
@@ -12584,13 +12527,13 @@
         <v>486</v>
       </c>
       <c r="B177" t="s">
-        <v>553</v>
+        <v>168</v>
       </c>
       <c r="C177" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="D177">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E177" t="s">
         <v>255</v>
@@ -12601,13 +12544,13 @@
         <v>487</v>
       </c>
       <c r="B178" t="s">
-        <v>554</v>
+        <v>169</v>
       </c>
       <c r="C178" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="D178">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E178" t="s">
         <v>255</v>
@@ -12618,13 +12561,13 @@
         <v>488</v>
       </c>
       <c r="B179" t="s">
-        <v>555</v>
+        <v>170</v>
       </c>
       <c r="C179" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="D179">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E179" t="s">
         <v>255</v>
@@ -12635,13 +12578,13 @@
         <v>489</v>
       </c>
       <c r="B180" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C180" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="D180">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E180" t="s">
         <v>255</v>
@@ -12652,13 +12595,13 @@
         <v>490</v>
       </c>
       <c r="B181" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="C181" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="D181">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E181" t="s">
         <v>255</v>
@@ -12669,13 +12612,13 @@
         <v>491</v>
       </c>
       <c r="B182" t="s">
-        <v>167</v>
+        <v>282</v>
       </c>
       <c r="C182" t="s">
         <v>230</v>
       </c>
       <c r="D182">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E182" t="s">
         <v>255</v>
@@ -12686,13 +12629,13 @@
         <v>492</v>
       </c>
       <c r="B183" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C183" t="s">
-        <v>230</v>
+        <v>192</v>
       </c>
       <c r="D183">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="E183" t="s">
         <v>255</v>
@@ -12703,13 +12646,13 @@
         <v>493</v>
       </c>
       <c r="B184" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C184" t="s">
-        <v>230</v>
+        <v>192</v>
       </c>
       <c r="D184">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="E184" t="s">
         <v>255</v>
@@ -12720,13 +12663,13 @@
         <v>494</v>
       </c>
       <c r="B185" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="C185" t="s">
-        <v>230</v>
+        <v>192</v>
       </c>
       <c r="D185">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="E185" t="s">
         <v>255</v>
@@ -12737,13 +12680,13 @@
         <v>495</v>
       </c>
       <c r="B186" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="C186" t="s">
-        <v>230</v>
+        <v>192</v>
       </c>
       <c r="D186">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="E186" t="s">
         <v>255</v>
@@ -12754,13 +12697,13 @@
         <v>496</v>
       </c>
       <c r="B187" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C187" t="s">
-        <v>230</v>
+        <v>192</v>
       </c>
       <c r="D187">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E187" t="s">
         <v>255</v>
@@ -12771,13 +12714,13 @@
         <v>497</v>
       </c>
       <c r="B188" t="s">
-        <v>282</v>
+        <v>178</v>
       </c>
       <c r="C188" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="D188">
-        <v>2021</v>
+        <v>2015</v>
       </c>
       <c r="E188" t="s">
         <v>255</v>
@@ -12788,13 +12731,13 @@
         <v>498</v>
       </c>
       <c r="B189" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C189" t="s">
-        <v>192</v>
+        <v>218</v>
       </c>
       <c r="D189">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E189" t="s">
         <v>255</v>
@@ -12805,13 +12748,13 @@
         <v>499</v>
       </c>
       <c r="B190" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C190" t="s">
-        <v>192</v>
+        <v>218</v>
       </c>
       <c r="D190">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E190" t="s">
         <v>255</v>
@@ -12822,13 +12765,13 @@
         <v>500</v>
       </c>
       <c r="B191" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C191" t="s">
-        <v>192</v>
+        <v>218</v>
       </c>
       <c r="D191">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E191" t="s">
         <v>255</v>
@@ -12839,13 +12782,13 @@
         <v>501</v>
       </c>
       <c r="B192" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="C192" t="s">
-        <v>192</v>
+        <v>218</v>
       </c>
       <c r="D192">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E192" t="s">
         <v>255</v>
@@ -12856,13 +12799,13 @@
         <v>502</v>
       </c>
       <c r="B193" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C193" t="s">
-        <v>192</v>
+        <v>218</v>
       </c>
       <c r="D193">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E193" t="s">
         <v>255</v>
@@ -12873,13 +12816,13 @@
         <v>503</v>
       </c>
       <c r="B194" t="s">
-        <v>178</v>
+        <v>280</v>
       </c>
       <c r="C194" t="s">
         <v>218</v>
       </c>
       <c r="D194">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E194" t="s">
         <v>255</v>
@@ -12890,13 +12833,13 @@
         <v>504</v>
       </c>
       <c r="B195" t="s">
-        <v>179</v>
+        <v>550</v>
       </c>
       <c r="C195" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="D195">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E195" t="s">
         <v>255</v>
@@ -12907,13 +12850,13 @@
         <v>505</v>
       </c>
       <c r="B196" t="s">
-        <v>180</v>
+        <v>551</v>
       </c>
       <c r="C196" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="D196">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E196" t="s">
         <v>255</v>
@@ -12924,13 +12867,13 @@
         <v>506</v>
       </c>
       <c r="B197" t="s">
-        <v>181</v>
+        <v>552</v>
       </c>
       <c r="C197" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="D197">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E197" t="s">
         <v>255</v>
@@ -12941,13 +12884,13 @@
         <v>507</v>
       </c>
       <c r="B198" t="s">
-        <v>182</v>
+        <v>553</v>
       </c>
       <c r="C198" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="D198">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E198" t="s">
         <v>255</v>
@@ -12958,13 +12901,13 @@
         <v>508</v>
       </c>
       <c r="B199" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C199" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="D199">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E199" t="s">
         <v>255</v>
@@ -12975,13 +12918,13 @@
         <v>509</v>
       </c>
       <c r="B200" t="s">
-        <v>280</v>
+        <v>189</v>
       </c>
       <c r="C200" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="D200">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E200" t="s">
         <v>255</v>
@@ -12992,122 +12935,20 @@
         <v>510</v>
       </c>
       <c r="B201" t="s">
-        <v>556</v>
+        <v>297</v>
       </c>
       <c r="C201" t="s">
         <v>210</v>
       </c>
       <c r="D201">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E201" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>511</v>
-      </c>
-      <c r="B202" t="s">
-        <v>557</v>
-      </c>
-      <c r="C202" t="s">
-        <v>210</v>
-      </c>
-      <c r="D202">
-        <v>2016</v>
-      </c>
-      <c r="E202" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
-        <v>512</v>
-      </c>
-      <c r="B203" t="s">
-        <v>558</v>
-      </c>
-      <c r="C203" t="s">
-        <v>210</v>
-      </c>
-      <c r="D203">
-        <v>2017</v>
-      </c>
-      <c r="E203" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
-        <v>513</v>
-      </c>
-      <c r="B204" t="s">
-        <v>559</v>
-      </c>
-      <c r="C204" t="s">
-        <v>210</v>
-      </c>
-      <c r="D204">
-        <v>2018</v>
-      </c>
-      <c r="E204" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
-        <v>514</v>
-      </c>
-      <c r="B205" t="s">
-        <v>188</v>
-      </c>
-      <c r="C205" t="s">
-        <v>210</v>
-      </c>
-      <c r="D205">
-        <v>2019</v>
-      </c>
-      <c r="E205" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>515</v>
-      </c>
-      <c r="B206" t="s">
-        <v>189</v>
-      </c>
-      <c r="C206" t="s">
-        <v>210</v>
-      </c>
-      <c r="D206">
-        <v>2020</v>
-      </c>
-      <c r="E206" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>516</v>
-      </c>
-      <c r="B207" t="s">
-        <v>297</v>
-      </c>
-      <c r="C207" t="s">
-        <v>210</v>
-      </c>
-      <c r="D207">
-        <v>2021</v>
-      </c>
-      <c r="E207" t="s">
-        <v>255</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E207" xr:uid="{1CCCF928-8895-4AB9-B900-2E463F961084}"/>
+  <autoFilter ref="A1:E201" xr:uid="{1CCCF928-8895-4AB9-B900-2E463F961084}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>